<commit_message>
Subida para mapear para o Jenkins
</commit_message>
<xml_diff>
--- a/public/migracao/clientes1.xlsx
+++ b/public/migracao/clientes1.xlsx
@@ -10,7 +10,7 @@
     <sheet sheetId="1" r:id="rId1" name="Clientes"/>
   </sheets>
   <definedNames>
-    <definedName name="Clientes">'Clientes'!$A$1:$AE$155</definedName>
+    <definedName name="Clientes">'Clientes'!$A$1:$AE$159</definedName>
   </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
@@ -347,7 +347,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE155"/>
+  <dimension ref="A1:AE159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -626,15 +626,15 @@
     </row>
     <row outlineLevel="0" r="6">
       <c r="A6" s="0">
-        <v>125</v>
+        <v>170</v>
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>ALTAMIR VAZ JUNIOR</t>
+          <t>AGÊNCIA TERRUÁ</t>
         </is>
       </c>
       <c r="V6" s="1">
-        <v>43828</v>
+        <v>44658</v>
       </c>
       <c r="W6" s="0">
         <v>0</v>
@@ -654,15 +654,15 @@
     </row>
     <row outlineLevel="0" r="7">
       <c r="A7" s="0">
-        <v>88</v>
+        <v>125</v>
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
-          <t>AMBEV</t>
+          <t>ALTAMIR VAZ JUNIOR</t>
         </is>
       </c>
       <c r="V7" s="1">
-        <v>43273</v>
+        <v>43828</v>
       </c>
       <c r="W7" s="0">
         <v>0</v>
@@ -682,15 +682,15 @@
     </row>
     <row outlineLevel="0" r="8">
       <c r="A8" s="0">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
-          <t>ANEXO RJ</t>
+          <t>AMBEV</t>
         </is>
       </c>
       <c r="V8" s="1">
-        <v>43051</v>
+        <v>43273</v>
       </c>
       <c r="W8" s="0">
         <v>0</v>
@@ -710,15 +710,15 @@
     </row>
     <row outlineLevel="0" r="9">
       <c r="A9" s="0">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t>AQUA RIO</t>
+          <t>ANEXO RJ</t>
         </is>
       </c>
       <c r="V9" s="1">
-        <v>43651</v>
+        <v>43051</v>
       </c>
       <c r="W9" s="0">
         <v>0</v>
@@ -738,20 +738,15 @@
     </row>
     <row outlineLevel="0" r="10">
       <c r="A10" s="0">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B10" s="0" t="inlineStr">
         <is>
-          <t>AT2D</t>
-        </is>
-      </c>
-      <c r="C10" s="0" t="inlineStr">
-        <is>
-          <t>PORSCHE</t>
+          <t>AQUA RIO</t>
         </is>
       </c>
       <c r="V10" s="1">
-        <v>43771</v>
+        <v>43651</v>
       </c>
       <c r="W10" s="0">
         <v>0</v>
@@ -771,15 +766,20 @@
     </row>
     <row outlineLevel="0" r="11">
       <c r="A11" s="0">
-        <v>146</v>
+        <v>116</v>
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
-          <t>B2W</t>
+          <t>AT2D</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>PORSCHE</t>
         </is>
       </c>
       <c r="V11" s="1">
-        <v>44321</v>
+        <v>43771</v>
       </c>
       <c r="W11" s="0">
         <v>0</v>
@@ -799,15 +799,15 @@
     </row>
     <row outlineLevel="0" r="12">
       <c r="A12" s="0">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="B12" s="0" t="inlineStr">
         <is>
-          <t>BACARDI</t>
+          <t>B2W</t>
         </is>
       </c>
       <c r="V12" s="1">
-        <v>44608</v>
+        <v>44321</v>
       </c>
       <c r="W12" s="0">
         <v>0</v>
@@ -827,15 +827,15 @@
     </row>
     <row outlineLevel="0" r="13">
       <c r="A13" s="0">
-        <v>85</v>
+        <v>166</v>
       </c>
       <c r="B13" s="0" t="inlineStr">
         <is>
-          <t>BDZ PRODUÇÕES</t>
+          <t>BACARDI</t>
         </is>
       </c>
       <c r="V13" s="1">
-        <v>43234</v>
+        <v>44608</v>
       </c>
       <c r="W13" s="0">
         <v>0</v>
@@ -855,15 +855,15 @@
     </row>
     <row outlineLevel="0" r="14">
       <c r="A14" s="0">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="B14" s="0" t="inlineStr">
         <is>
-          <t>BELUGA</t>
+          <t>BDZ PRODUÇÕES</t>
         </is>
       </c>
       <c r="V14" s="1">
-        <v>42670</v>
+        <v>43234</v>
       </c>
       <c r="W14" s="0">
         <v>0</v>
@@ -883,15 +883,15 @@
     </row>
     <row outlineLevel="0" r="15">
       <c r="A15" s="0">
-        <v>54</v>
+        <v>172</v>
       </c>
       <c r="B15" s="0" t="inlineStr">
         <is>
-          <t>BRASA FOODIES</t>
+          <t>BE COMUNICA</t>
         </is>
       </c>
       <c r="V15" s="1">
-        <v>42677</v>
+        <v>44669</v>
       </c>
       <c r="W15" s="0">
         <v>0</v>
@@ -911,15 +911,15 @@
     </row>
     <row outlineLevel="0" r="16">
       <c r="A16" s="0">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B16" s="0" t="inlineStr">
         <is>
-          <t>BRMALLS</t>
+          <t>BELUGA</t>
         </is>
       </c>
       <c r="V16" s="1">
-        <v>42545</v>
+        <v>42670</v>
       </c>
       <c r="W16" s="0">
         <v>0</v>
@@ -939,15 +939,15 @@
     </row>
     <row outlineLevel="0" r="17">
       <c r="A17" s="0">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="B17" s="0" t="inlineStr">
         <is>
-          <t>BRUNO BEZERRA</t>
+          <t>BRASA FOODIES</t>
         </is>
       </c>
       <c r="V17" s="1">
-        <v>42446</v>
+        <v>42677</v>
       </c>
       <c r="W17" s="0">
         <v>0</v>
@@ -967,15 +967,15 @@
     </row>
     <row outlineLevel="0" r="18">
       <c r="A18" s="0">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B18" s="0" t="inlineStr">
         <is>
-          <t>BRUNO LANDEIRA</t>
+          <t>BRMALLS</t>
         </is>
       </c>
       <c r="V18" s="1">
-        <v>42241</v>
+        <v>42545</v>
       </c>
       <c r="W18" s="0">
         <v>0</v>
@@ -995,15 +995,15 @@
     </row>
     <row outlineLevel="0" r="19">
       <c r="A19" s="0">
-        <v>123</v>
+        <v>36</v>
       </c>
       <c r="B19" s="0" t="inlineStr">
         <is>
-          <t>BRUNO MEROLLA</t>
+          <t>BRUNO BEZERRA</t>
         </is>
       </c>
       <c r="V19" s="1">
-        <v>43819</v>
+        <v>42446</v>
       </c>
       <c r="W19" s="0">
         <v>0</v>
@@ -1023,15 +1023,15 @@
     </row>
     <row outlineLevel="0" r="20">
       <c r="A20" s="0">
-        <v>158</v>
+        <v>20</v>
       </c>
       <c r="B20" s="0" t="inlineStr">
         <is>
-          <t>CACO DE VIDRO</t>
+          <t>BRUNO LANDEIRA</t>
         </is>
       </c>
       <c r="V20" s="1">
-        <v>44475</v>
+        <v>42241</v>
       </c>
       <c r="W20" s="0">
         <v>0</v>
@@ -1051,15 +1051,15 @@
     </row>
     <row outlineLevel="0" r="21">
       <c r="A21" s="0">
-        <v>83</v>
+        <v>123</v>
       </c>
       <c r="B21" s="0" t="inlineStr">
         <is>
-          <t>CAMAROTE ALEGRIA 2018</t>
+          <t>BRUNO MEROLLA</t>
         </is>
       </c>
       <c r="V21" s="1">
-        <v>43122</v>
+        <v>43819</v>
       </c>
       <c r="W21" s="0">
         <v>0</v>
@@ -1079,15 +1079,15 @@
     </row>
     <row outlineLevel="0" r="22">
       <c r="A22" s="0">
-        <v>96</v>
+        <v>158</v>
       </c>
       <c r="B22" s="0" t="inlineStr">
         <is>
-          <t>CAMAROTE RIO</t>
+          <t>CACO DE VIDRO</t>
         </is>
       </c>
       <c r="V22" s="1">
-        <v>43522</v>
+        <v>44475</v>
       </c>
       <c r="W22" s="0">
         <v>0</v>
@@ -1107,15 +1107,15 @@
     </row>
     <row outlineLevel="0" r="23">
       <c r="A23" s="0">
-        <v>26</v>
+        <v>83</v>
       </c>
       <c r="B23" s="0" t="inlineStr">
         <is>
-          <t>CANAL OFF</t>
+          <t>CAMAROTE ALEGRIA 2018</t>
         </is>
       </c>
       <c r="V23" s="1">
-        <v>42337</v>
+        <v>43122</v>
       </c>
       <c r="W23" s="0">
         <v>0</v>
@@ -1135,15 +1135,15 @@
     </row>
     <row outlineLevel="0" r="24">
       <c r="A24" s="0">
-        <v>144</v>
+        <v>96</v>
       </c>
       <c r="B24" s="0" t="inlineStr">
         <is>
-          <t>CASTAS</t>
+          <t>CAMAROTE RIO</t>
         </is>
       </c>
       <c r="V24" s="1">
-        <v>44314</v>
+        <v>43522</v>
       </c>
       <c r="W24" s="0">
         <v>0</v>
@@ -1163,15 +1163,15 @@
     </row>
     <row outlineLevel="0" r="25">
       <c r="A25" s="0">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B25" s="0" t="inlineStr">
         <is>
-          <t>CB PRODUÇÕES</t>
+          <t>CANAL OFF</t>
         </is>
       </c>
       <c r="V25" s="1">
-        <v>42432</v>
+        <v>42337</v>
       </c>
       <c r="W25" s="0">
         <v>0</v>
@@ -1191,15 +1191,15 @@
     </row>
     <row outlineLevel="0" r="26">
       <c r="A26" s="0">
-        <v>47</v>
+        <v>144</v>
       </c>
       <c r="B26" s="0" t="inlineStr">
         <is>
-          <t>CERVEJARIA  PRAYA</t>
+          <t>CASTAS</t>
         </is>
       </c>
       <c r="V26" s="1">
-        <v>42621</v>
+        <v>44314</v>
       </c>
       <c r="W26" s="0">
         <v>0</v>
@@ -1219,15 +1219,15 @@
     </row>
     <row outlineLevel="0" r="27">
       <c r="A27" s="0">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B27" s="0" t="inlineStr">
         <is>
-          <t>CERVEJARIA PRAYA</t>
+          <t>CB PRODUÇÕES</t>
         </is>
       </c>
       <c r="V27" s="1">
-        <v>42523</v>
+        <v>42432</v>
       </c>
       <c r="W27" s="0">
         <v>0</v>
@@ -1247,15 +1247,15 @@
     </row>
     <row outlineLevel="0" r="28">
       <c r="A28" s="0">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B28" s="0" t="inlineStr">
         <is>
-          <t>CERVEJARIA TEREZÓPOLIS</t>
+          <t>CERVEJARIA  PRAYA</t>
         </is>
       </c>
       <c r="V28" s="1">
-        <v>42881</v>
+        <v>42621</v>
       </c>
       <c r="W28" s="0">
         <v>0</v>
@@ -1275,15 +1275,15 @@
     </row>
     <row outlineLevel="0" r="29">
       <c r="A29" s="0">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="B29" s="0" t="inlineStr">
         <is>
-          <t>CHIQUINHO - TOTO</t>
+          <t>CERVEJARIA PRAYA</t>
         </is>
       </c>
       <c r="V29" s="1">
-        <v>42956</v>
+        <v>42523</v>
       </c>
       <c r="W29" s="0">
         <v>0</v>
@@ -1303,15 +1303,15 @@
     </row>
     <row outlineLevel="0" r="30">
       <c r="A30" s="0">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B30" s="0" t="inlineStr">
         <is>
-          <t>CIA MULLER DE BEBIDAS</t>
+          <t>CERVEJARIA TEREZÓPOLIS</t>
         </is>
       </c>
       <c r="V30" s="1">
-        <v>42992</v>
+        <v>42881</v>
       </c>
       <c r="W30" s="0">
         <v>0</v>
@@ -1331,15 +1331,15 @@
     </row>
     <row outlineLevel="0" r="31">
       <c r="A31" s="0">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="B31" s="0" t="inlineStr">
         <is>
-          <t>CLEAR CHANNEL</t>
+          <t>CHIQUINHO - TOTO</t>
         </is>
       </c>
       <c r="V31" s="1">
-        <v>42554</v>
+        <v>42956</v>
       </c>
       <c r="W31" s="0">
         <v>0</v>
@@ -1359,15 +1359,15 @@
     </row>
     <row outlineLevel="0" r="32">
       <c r="A32" s="0">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="B32" s="0" t="inlineStr">
         <is>
-          <t>COOL PRODUÇÕES</t>
+          <t>CIA MULLER DE BEBIDAS</t>
         </is>
       </c>
       <c r="V32" s="1">
-        <v>42466</v>
+        <v>42992</v>
       </c>
       <c r="W32" s="0">
         <v>0</v>
@@ -1387,15 +1387,15 @@
     </row>
     <row outlineLevel="0" r="33">
       <c r="A33" s="0">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B33" s="0" t="inlineStr">
         <is>
-          <t>CRIAATVA</t>
+          <t>CLEAR CHANNEL</t>
         </is>
       </c>
       <c r="V33" s="1">
-        <v>42171</v>
+        <v>42554</v>
       </c>
       <c r="W33" s="0">
         <v>0</v>
@@ -1415,15 +1415,15 @@
     </row>
     <row outlineLevel="0" r="34">
       <c r="A34" s="0">
-        <v>91</v>
+        <v>38</v>
       </c>
       <c r="B34" s="0" t="inlineStr">
         <is>
-          <t>CS EVENTOS</t>
+          <t>COOL PRODUÇÕES</t>
         </is>
       </c>
       <c r="V34" s="1">
-        <v>43354</v>
+        <v>42466</v>
       </c>
       <c r="W34" s="0">
         <v>0</v>
@@ -1443,15 +1443,15 @@
     </row>
     <row outlineLevel="0" r="35">
       <c r="A35" s="0">
-        <v>152</v>
+        <v>11</v>
       </c>
       <c r="B35" s="0" t="inlineStr">
         <is>
-          <t>D2S SERVIÇO DE SEGURANÇA</t>
+          <t>CRIAATVA</t>
         </is>
       </c>
       <c r="V35" s="1">
-        <v>44405</v>
+        <v>42171</v>
       </c>
       <c r="W35" s="0">
         <v>0</v>
@@ -1471,15 +1471,15 @@
     </row>
     <row outlineLevel="0" r="36">
       <c r="A36" s="0">
-        <v>155</v>
+        <v>91</v>
       </c>
       <c r="B36" s="0" t="inlineStr">
         <is>
-          <t>DANI SOLON</t>
+          <t>CS EVENTOS</t>
         </is>
       </c>
       <c r="V36" s="1">
-        <v>44447</v>
+        <v>43354</v>
       </c>
       <c r="W36" s="0">
         <v>0</v>
@@ -1499,15 +1499,15 @@
     </row>
     <row outlineLevel="0" r="37">
       <c r="A37" s="0">
-        <v>61</v>
+        <v>152</v>
       </c>
       <c r="B37" s="0" t="inlineStr">
         <is>
-          <t>DELETADA</t>
+          <t>D2S SERVIÇO DE SEGURANÇA</t>
         </is>
       </c>
       <c r="V37" s="1">
-        <v>42802</v>
+        <v>44405</v>
       </c>
       <c r="W37" s="0">
         <v>0</v>
@@ -1527,15 +1527,15 @@
     </row>
     <row outlineLevel="0" r="38">
       <c r="A38" s="0">
-        <v>76</v>
+        <v>155</v>
       </c>
       <c r="B38" s="0" t="inlineStr">
         <is>
-          <t>DIAGEO</t>
+          <t>DANI SOLON</t>
         </is>
       </c>
       <c r="V38" s="1">
-        <v>43007</v>
+        <v>44447</v>
       </c>
       <c r="W38" s="0">
         <v>0</v>
@@ -1555,15 +1555,15 @@
     </row>
     <row outlineLevel="0" r="39">
       <c r="A39" s="0">
-        <v>156</v>
+        <v>61</v>
       </c>
       <c r="B39" s="0" t="inlineStr">
         <is>
-          <t>DIALOGO URBANO - BARBARA SOLEDADE</t>
+          <t>DELETADA</t>
         </is>
       </c>
       <c r="V39" s="1">
-        <v>44448</v>
+        <v>42802</v>
       </c>
       <c r="W39" s="0">
         <v>0</v>
@@ -1583,15 +1583,15 @@
     </row>
     <row outlineLevel="0" r="40">
       <c r="A40" s="0">
-        <v>157</v>
+        <v>76</v>
       </c>
       <c r="B40" s="0" t="inlineStr">
         <is>
-          <t>DION ME</t>
+          <t>DIAGEO</t>
         </is>
       </c>
       <c r="V40" s="1">
-        <v>44452</v>
+        <v>43007</v>
       </c>
       <c r="W40" s="0">
         <v>0</v>
@@ -1611,15 +1611,15 @@
     </row>
     <row outlineLevel="0" r="41">
       <c r="A41" s="0">
-        <v>63</v>
+        <v>156</v>
       </c>
       <c r="B41" s="0" t="inlineStr">
         <is>
-          <t>DOMINUS - BRAMEX</t>
+          <t>DIALOGO URBANO - BARBARA SOLEDADE</t>
         </is>
       </c>
       <c r="V41" s="1">
-        <v>42831</v>
+        <v>44448</v>
       </c>
       <c r="W41" s="0">
         <v>0</v>
@@ -1639,15 +1639,15 @@
     </row>
     <row outlineLevel="0" r="42">
       <c r="A42" s="0">
-        <v>105</v>
+        <v>157</v>
       </c>
       <c r="B42" s="0" t="inlineStr">
         <is>
-          <t>DREAM FACTORY</t>
+          <t>DION ME</t>
         </is>
       </c>
       <c r="V42" s="1">
-        <v>43633</v>
+        <v>44452</v>
       </c>
       <c r="W42" s="0">
         <v>0</v>
@@ -1667,15 +1667,15 @@
     </row>
     <row outlineLevel="0" r="43">
       <c r="A43" s="0">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="B43" s="0" t="inlineStr">
         <is>
-          <t>DUDA GASPAR</t>
+          <t>DOMINUS - BRAMEX</t>
         </is>
       </c>
       <c r="V43" s="1">
-        <v>42200</v>
+        <v>42831</v>
       </c>
       <c r="W43" s="0">
         <v>0</v>
@@ -1695,15 +1695,15 @@
     </row>
     <row outlineLevel="0" r="44">
       <c r="A44" s="0">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B44" s="0" t="inlineStr">
         <is>
-          <t>ELEMENTAL 5</t>
+          <t>DREAM FACTORY</t>
         </is>
       </c>
       <c r="V44" s="1">
-        <v>43579</v>
+        <v>43633</v>
       </c>
       <c r="W44" s="0">
         <v>0</v>
@@ -1723,15 +1723,15 @@
     </row>
     <row outlineLevel="0" r="45">
       <c r="A45" s="0">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="B45" s="0" t="inlineStr">
         <is>
-          <t>ESCOLA ELEVA</t>
+          <t>DUDA GASPAR</t>
         </is>
       </c>
       <c r="V45" s="1">
-        <v>42885</v>
+        <v>42200</v>
       </c>
       <c r="W45" s="0">
         <v>0</v>
@@ -1751,15 +1751,15 @@
     </row>
     <row outlineLevel="0" r="46">
       <c r="A46" s="0">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="B46" s="0" t="inlineStr">
         <is>
-          <t>FÁBRICA</t>
+          <t>ELEMENTAL 5</t>
         </is>
       </c>
       <c r="V46" s="1">
-        <v>43805</v>
+        <v>43579</v>
       </c>
       <c r="W46" s="0">
         <v>0</v>
@@ -1779,15 +1779,15 @@
     </row>
     <row outlineLevel="0" r="47">
       <c r="A47" s="0">
-        <v>142</v>
+        <v>70</v>
       </c>
       <c r="B47" s="0" t="inlineStr">
         <is>
-          <t>FÁBRICA.AG</t>
+          <t>ESCOLA ELEVA</t>
         </is>
       </c>
       <c r="V47" s="1">
-        <v>44280</v>
+        <v>42885</v>
       </c>
       <c r="W47" s="0">
         <v>0</v>
@@ -1807,15 +1807,15 @@
     </row>
     <row outlineLevel="0" r="48">
       <c r="A48" s="0">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="B48" s="0" t="inlineStr">
         <is>
-          <t>FABRÍCIO STOFEL</t>
+          <t>FÁBRICA</t>
         </is>
       </c>
       <c r="V48" s="1">
-        <v>43248</v>
+        <v>43805</v>
       </c>
       <c r="W48" s="0">
         <v>0</v>
@@ -1835,15 +1835,15 @@
     </row>
     <row outlineLevel="0" r="49">
       <c r="A49" s="0">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="B49" s="0" t="inlineStr">
         <is>
-          <t>FAIRMONT</t>
+          <t>FÁBRICA.AG</t>
         </is>
       </c>
       <c r="V49" s="1">
-        <v>44161</v>
+        <v>44280</v>
       </c>
       <c r="W49" s="0">
         <v>0</v>
@@ -1863,15 +1863,15 @@
     </row>
     <row outlineLevel="0" r="50">
       <c r="A50" s="0">
-        <v>58</v>
+        <v>87</v>
       </c>
       <c r="B50" s="0" t="inlineStr">
         <is>
-          <t>FARM</t>
+          <t>FABRÍCIO STOFEL</t>
         </is>
       </c>
       <c r="V50" s="1">
-        <v>42754</v>
+        <v>43248</v>
       </c>
       <c r="W50" s="0">
         <v>0</v>
@@ -1891,15 +1891,15 @@
     </row>
     <row outlineLevel="0" r="51">
       <c r="A51" s="0">
-        <v>95</v>
+        <v>135</v>
       </c>
       <c r="B51" s="0" t="inlineStr">
         <is>
-          <t>FELIPE BITTENCOURT</t>
+          <t>FAIRMONT</t>
         </is>
       </c>
       <c r="V51" s="1">
-        <v>43520</v>
+        <v>44161</v>
       </c>
       <c r="W51" s="0">
         <v>0</v>
@@ -1919,15 +1919,15 @@
     </row>
     <row outlineLevel="0" r="52">
       <c r="A52" s="0">
-        <v>161</v>
+        <v>58</v>
       </c>
       <c r="B52" s="0" t="inlineStr">
         <is>
-          <t>FLYSPORTS</t>
+          <t>FARM</t>
         </is>
       </c>
       <c r="V52" s="1">
-        <v>44483</v>
+        <v>42754</v>
       </c>
       <c r="W52" s="0">
         <v>0</v>
@@ -1947,15 +1947,15 @@
     </row>
     <row outlineLevel="0" r="53">
       <c r="A53" s="0">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="B53" s="0" t="inlineStr">
         <is>
-          <t>FOODIES</t>
+          <t>FELIPE BITTENCOURT</t>
         </is>
       </c>
       <c r="V53" s="1">
-        <v>42475</v>
+        <v>43520</v>
       </c>
       <c r="W53" s="0">
         <v>0</v>
@@ -1975,15 +1975,15 @@
     </row>
     <row outlineLevel="0" r="54">
       <c r="A54" s="0">
-        <v>50</v>
+        <v>161</v>
       </c>
       <c r="B54" s="0" t="inlineStr">
         <is>
-          <t>FOXTON</t>
+          <t>FLYSPORTS</t>
         </is>
       </c>
       <c r="V54" s="1">
-        <v>42649</v>
+        <v>44483</v>
       </c>
       <c r="W54" s="0">
         <v>0</v>
@@ -2003,15 +2003,15 @@
     </row>
     <row outlineLevel="0" r="55">
       <c r="A55" s="0">
-        <v>148</v>
+        <v>40</v>
       </c>
       <c r="B55" s="0" t="inlineStr">
         <is>
-          <t>GENEAL</t>
+          <t>FOODIES</t>
         </is>
       </c>
       <c r="V55" s="1">
-        <v>44363</v>
+        <v>42475</v>
       </c>
       <c r="W55" s="0">
         <v>0</v>
@@ -2031,15 +2031,15 @@
     </row>
     <row outlineLevel="0" r="56">
       <c r="A56" s="0">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B56" s="0" t="inlineStr">
         <is>
-          <t>GLOBO SAT</t>
+          <t>FOXTON</t>
         </is>
       </c>
       <c r="V56" s="1">
-        <v>42656</v>
+        <v>42649</v>
       </c>
       <c r="W56" s="0">
         <v>0</v>
@@ -2059,15 +2059,15 @@
     </row>
     <row outlineLevel="0" r="57">
       <c r="A57" s="0">
-        <v>121</v>
+        <v>148</v>
       </c>
       <c r="B57" s="0" t="inlineStr">
         <is>
-          <t>GLOBOPLAY</t>
+          <t>GENEAL</t>
         </is>
       </c>
       <c r="V57" s="1">
-        <v>43817</v>
+        <v>44363</v>
       </c>
       <c r="W57" s="0">
         <v>0</v>
@@ -2087,15 +2087,30 @@
     </row>
     <row outlineLevel="0" r="58">
       <c r="A58" s="0">
-        <v>25</v>
+        <v>171</v>
       </c>
       <c r="B58" s="0" t="inlineStr">
         <is>
-          <t>GMP</t>
+          <t>GLOBO COMUNICAÇÕES</t>
+        </is>
+      </c>
+      <c r="F58" s="0" t="inlineStr">
+        <is>
+          <t>RUA LOPES QUINTTAS, 303</t>
+        </is>
+      </c>
+      <c r="G58" s="0" t="inlineStr">
+        <is>
+          <t>JARDIM BOTANICO</t>
+        </is>
+      </c>
+      <c r="L58" s="0" t="inlineStr">
+        <is>
+          <t>27.865.757/0001-02</t>
         </is>
       </c>
       <c r="V58" s="1">
-        <v>42334</v>
+        <v>44669</v>
       </c>
       <c r="W58" s="0">
         <v>0</v>
@@ -2115,15 +2130,15 @@
     </row>
     <row outlineLevel="0" r="59">
       <c r="A59" s="0">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B59" s="0" t="inlineStr">
         <is>
-          <t>GRUPO 8</t>
+          <t>GLOBO SAT</t>
         </is>
       </c>
       <c r="V59" s="1">
-        <v>42453</v>
+        <v>42656</v>
       </c>
       <c r="W59" s="0">
         <v>0</v>
@@ -2143,15 +2158,15 @@
     </row>
     <row outlineLevel="0" r="60">
       <c r="A60" s="0">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="B60" s="0" t="inlineStr">
         <is>
-          <t>GRUPO CATARATAS</t>
+          <t>GLOBOPLAY</t>
         </is>
       </c>
       <c r="V60" s="1">
-        <v>43596</v>
+        <v>43817</v>
       </c>
       <c r="W60" s="0">
         <v>0</v>
@@ -2171,15 +2186,15 @@
     </row>
     <row outlineLevel="0" r="61">
       <c r="A61" s="0">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="B61" s="0" t="inlineStr">
         <is>
-          <t>HANDRED</t>
+          <t>GMP</t>
         </is>
       </c>
       <c r="V61" s="1">
-        <v>42872</v>
+        <v>42334</v>
       </c>
       <c r="W61" s="0">
         <v>0</v>
@@ -2199,15 +2214,15 @@
     </row>
     <row outlineLevel="0" r="62">
       <c r="A62" s="0">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="B62" s="0" t="inlineStr">
         <is>
-          <t>HARRISON</t>
+          <t>GRUPO 8</t>
         </is>
       </c>
       <c r="V62" s="1">
-        <v>42165</v>
+        <v>42453</v>
       </c>
       <c r="W62" s="0">
         <v>0</v>
@@ -2227,15 +2242,15 @@
     </row>
     <row outlineLevel="0" r="63">
       <c r="A63" s="0">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B63" s="0" t="inlineStr">
         <is>
-          <t>HAUTE</t>
+          <t>GRUPO CATARATAS</t>
         </is>
       </c>
       <c r="V63" s="1">
-        <v>43720</v>
+        <v>43596</v>
       </c>
       <c r="W63" s="0">
         <v>0</v>
@@ -2255,15 +2270,15 @@
     </row>
     <row outlineLevel="0" r="64">
       <c r="A64" s="0">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="B64" s="0" t="inlineStr">
         <is>
-          <t>HEADS</t>
+          <t>HANDRED</t>
         </is>
       </c>
       <c r="V64" s="1">
-        <v>43399</v>
+        <v>42872</v>
       </c>
       <c r="W64" s="0">
         <v>0</v>
@@ -2283,15 +2298,15 @@
     </row>
     <row outlineLevel="0" r="65">
       <c r="A65" s="0">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B65" s="0" t="inlineStr">
         <is>
-          <t>HEINEKEN</t>
+          <t>HARRISON</t>
         </is>
       </c>
       <c r="V65" s="1">
-        <v>42133</v>
+        <v>42165</v>
       </c>
       <c r="W65" s="0">
         <v>0</v>
@@ -2311,15 +2326,15 @@
     </row>
     <row outlineLevel="0" r="66">
       <c r="A66" s="0">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="B66" s="0" t="inlineStr">
         <is>
-          <t>HUB BRASIL</t>
+          <t>HAUTE</t>
         </is>
       </c>
       <c r="V66" s="1">
-        <v>43238</v>
+        <v>43720</v>
       </c>
       <c r="W66" s="0">
         <v>0</v>
@@ -2339,15 +2354,15 @@
     </row>
     <row outlineLevel="0" r="67">
       <c r="A67" s="0">
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="B67" s="0" t="inlineStr">
         <is>
-          <t>HUG ENTRETERIMENTO</t>
+          <t>HEADS</t>
         </is>
       </c>
       <c r="V67" s="1">
-        <v>42780</v>
+        <v>43399</v>
       </c>
       <c r="W67" s="0">
         <v>0</v>
@@ -2367,15 +2382,15 @@
     </row>
     <row outlineLevel="0" r="68">
       <c r="A68" s="0">
-        <v>131</v>
+        <v>4</v>
       </c>
       <c r="B68" s="0" t="inlineStr">
         <is>
-          <t>IABAS</t>
+          <t>HEINEKEN</t>
         </is>
       </c>
       <c r="V68" s="1">
-        <v>43937</v>
+        <v>42133</v>
       </c>
       <c r="W68" s="0">
         <v>0</v>
@@ -2395,15 +2410,15 @@
     </row>
     <row outlineLevel="0" r="69">
       <c r="A69" s="0">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="B69" s="0" t="inlineStr">
         <is>
-          <t>IDBR</t>
+          <t>HUB BRASIL</t>
         </is>
       </c>
       <c r="V69" s="1">
-        <v>43595</v>
+        <v>43238</v>
       </c>
       <c r="W69" s="0">
         <v>0</v>
@@ -2423,15 +2438,15 @@
     </row>
     <row outlineLevel="0" r="70">
       <c r="A70" s="0">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="B70" s="0" t="inlineStr">
         <is>
-          <t>IFOOD</t>
+          <t>HUG ENTRETERIMENTO</t>
         </is>
       </c>
       <c r="V70" s="1">
-        <v>44575</v>
+        <v>42780</v>
       </c>
       <c r="W70" s="0">
         <v>0</v>
@@ -2451,15 +2466,15 @@
     </row>
     <row outlineLevel="0" r="71">
       <c r="A71" s="0">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B71" s="0" t="inlineStr">
         <is>
-          <t>INFOVIEW</t>
+          <t>IABAS</t>
         </is>
       </c>
       <c r="V71" s="1">
-        <v>44223</v>
+        <v>43937</v>
       </c>
       <c r="W71" s="0">
         <v>0</v>
@@ -2479,15 +2494,15 @@
     </row>
     <row outlineLevel="0" r="72">
       <c r="A72" s="0">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="B72" s="0" t="inlineStr">
         <is>
-          <t>ITAIPAVA</t>
+          <t>IDBR</t>
         </is>
       </c>
       <c r="V72" s="1">
-        <v>42117</v>
+        <v>43595</v>
       </c>
       <c r="W72" s="0">
         <v>0</v>
@@ -2507,15 +2522,15 @@
     </row>
     <row outlineLevel="0" r="73">
       <c r="A73" s="0">
-        <v>10</v>
+        <v>165</v>
       </c>
       <c r="B73" s="0" t="inlineStr">
         <is>
-          <t>ITAU</t>
+          <t>IFOOD</t>
         </is>
       </c>
       <c r="V73" s="1">
-        <v>42171</v>
+        <v>44575</v>
       </c>
       <c r="W73" s="0">
         <v>0</v>
@@ -2535,15 +2550,15 @@
     </row>
     <row outlineLevel="0" r="74">
       <c r="A74" s="0">
-        <v>102</v>
+        <v>138</v>
       </c>
       <c r="B74" s="0" t="inlineStr">
         <is>
-          <t>JONATHAS - WEB (PROCESSO)</t>
+          <t>INFOVIEW</t>
         </is>
       </c>
       <c r="V74" s="1">
-        <v>43593</v>
+        <v>44223</v>
       </c>
       <c r="W74" s="0">
         <v>0</v>
@@ -2563,15 +2578,15 @@
     </row>
     <row outlineLevel="0" r="75">
       <c r="A75" s="0">
-        <v>82</v>
+        <v>1</v>
       </c>
       <c r="B75" s="0" t="inlineStr">
         <is>
-          <t>LANDEIRA</t>
+          <t>ITAIPAVA</t>
         </is>
       </c>
       <c r="V75" s="1">
-        <v>43067</v>
+        <v>42117</v>
       </c>
       <c r="W75" s="0">
         <v>0</v>
@@ -2591,15 +2606,15 @@
     </row>
     <row outlineLevel="0" r="76">
       <c r="A76" s="0">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="B76" s="0" t="inlineStr">
         <is>
-          <t>LOWES</t>
+          <t>ITAU</t>
         </is>
       </c>
       <c r="V76" s="1">
-        <v>42678</v>
+        <v>42171</v>
       </c>
       <c r="W76" s="0">
         <v>0</v>
@@ -2619,15 +2634,15 @@
     </row>
     <row outlineLevel="0" r="77">
       <c r="A77" s="0">
-        <v>18</v>
+        <v>102</v>
       </c>
       <c r="B77" s="0" t="inlineStr">
         <is>
-          <t>LUCCE</t>
+          <t>JONATHAS - WEB (PROCESSO)</t>
         </is>
       </c>
       <c r="V77" s="1">
-        <v>42220</v>
+        <v>43593</v>
       </c>
       <c r="W77" s="0">
         <v>0</v>
@@ -2647,15 +2662,15 @@
     </row>
     <row outlineLevel="0" r="78">
       <c r="A78" s="0">
-        <v>134</v>
+        <v>82</v>
       </c>
       <c r="B78" s="0" t="inlineStr">
         <is>
-          <t>LUFE</t>
+          <t>LANDEIRA</t>
         </is>
       </c>
       <c r="V78" s="1">
-        <v>44154</v>
+        <v>43067</v>
       </c>
       <c r="W78" s="0">
         <v>0</v>
@@ -2675,15 +2690,15 @@
     </row>
     <row outlineLevel="0" r="79">
       <c r="A79" s="0">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B79" s="0" t="inlineStr">
         <is>
-          <t>LUIZ AMARAL</t>
+          <t>LOWES</t>
         </is>
       </c>
       <c r="V79" s="1">
-        <v>42724</v>
+        <v>42678</v>
       </c>
       <c r="W79" s="0">
         <v>0</v>
@@ -2703,15 +2718,15 @@
     </row>
     <row outlineLevel="0" r="80">
       <c r="A80" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B80" s="0" t="inlineStr">
         <is>
-          <t>LVHM</t>
+          <t>LUCCE</t>
         </is>
       </c>
       <c r="V80" s="1">
-        <v>42193</v>
+        <v>42220</v>
       </c>
       <c r="W80" s="0">
         <v>0</v>
@@ -2731,15 +2746,15 @@
     </row>
     <row outlineLevel="0" r="81">
       <c r="A81" s="0">
-        <v>27</v>
+        <v>134</v>
       </c>
       <c r="B81" s="0" t="inlineStr">
         <is>
-          <t>LVMH</t>
+          <t>LUFE</t>
         </is>
       </c>
       <c r="V81" s="1">
-        <v>42355</v>
+        <v>44154</v>
       </c>
       <c r="W81" s="0">
         <v>0</v>
@@ -2759,15 +2774,15 @@
     </row>
     <row outlineLevel="0" r="82">
       <c r="A82" s="0">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="B82" s="0" t="inlineStr">
         <is>
-          <t>MALAKA</t>
+          <t>LUIZ AMARAL</t>
         </is>
       </c>
       <c r="V82" s="1">
-        <v>42117</v>
+        <v>42724</v>
       </c>
       <c r="W82" s="0">
         <v>0</v>
@@ -2787,15 +2802,15 @@
     </row>
     <row outlineLevel="0" r="83">
       <c r="A83" s="0">
-        <v>167</v>
+        <v>16</v>
       </c>
       <c r="B83" s="0" t="inlineStr">
         <is>
-          <t>MARINA GIN</t>
+          <t>LVHM</t>
         </is>
       </c>
       <c r="V83" s="1">
-        <v>44616</v>
+        <v>42193</v>
       </c>
       <c r="W83" s="0">
         <v>0</v>
@@ -2815,15 +2830,15 @@
     </row>
     <row outlineLevel="0" r="84">
       <c r="A84" s="0">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B84" s="0" t="inlineStr">
         <is>
-          <t>METRÓPOLE</t>
+          <t>LVMH</t>
         </is>
       </c>
       <c r="V84" s="1">
-        <v>42242</v>
+        <v>42355</v>
       </c>
       <c r="W84" s="0">
         <v>0</v>
@@ -2843,15 +2858,15 @@
     </row>
     <row outlineLevel="0" r="85">
       <c r="A85" s="0">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="B85" s="0" t="inlineStr">
         <is>
-          <t>MOET HENNESSY</t>
+          <t>MALAKA</t>
         </is>
       </c>
       <c r="V85" s="1">
-        <v>42446</v>
+        <v>42117</v>
       </c>
       <c r="W85" s="0">
         <v>0</v>
@@ -2871,60 +2886,15 @@
     </row>
     <row outlineLevel="0" r="86">
       <c r="A86" s="0">
-        <v>99</v>
+        <v>167</v>
       </c>
       <c r="B86" s="0" t="inlineStr">
         <is>
-          <t>MOSTARDA PRODUÇÕES E EVENTOS LTDA - ME</t>
-        </is>
-      </c>
-      <c r="C86" s="0" t="inlineStr">
-        <is>
-          <t>MOSTARDA PRODUÇOES</t>
-        </is>
-      </c>
-      <c r="F86" s="0" t="inlineStr">
-        <is>
-          <t>RUA LEANDRO MARTINS, 10 SALA 902</t>
-        </is>
-      </c>
-      <c r="G86" s="0" t="inlineStr">
-        <is>
-          <t>CENTRO</t>
-        </is>
-      </c>
-      <c r="H86" s="0" t="inlineStr">
-        <is>
-          <t>RIO DE JANEIRO</t>
-        </is>
-      </c>
-      <c r="I86" s="0" t="inlineStr">
-        <is>
-          <t>RJ</t>
-        </is>
-      </c>
-      <c r="J86" s="0" t="inlineStr">
-        <is>
-          <t>20080-070</t>
-        </is>
-      </c>
-      <c r="L86" s="0" t="inlineStr">
-        <is>
-          <t>18.381.709/0001-40</t>
-        </is>
-      </c>
-      <c r="M86" s="0" t="inlineStr">
-        <is>
-          <t>ISENTO</t>
-        </is>
-      </c>
-      <c r="N86" s="0" t="inlineStr">
-        <is>
-          <t>0.582.179-7</t>
+          <t>MARINA GIN</t>
         </is>
       </c>
       <c r="V86" s="1">
-        <v>43560</v>
+        <v>44616</v>
       </c>
       <c r="W86" s="0">
         <v>0</v>
@@ -2944,20 +2914,15 @@
     </row>
     <row outlineLevel="0" r="87">
       <c r="A87" s="0">
-        <v>119</v>
+        <v>21</v>
       </c>
       <c r="B87" s="0" t="inlineStr">
         <is>
-          <t>NATHÁLIA QUINTANS</t>
-        </is>
-      </c>
-      <c r="O87" s="0" t="inlineStr">
-        <is>
-          <t>11010906771</t>
+          <t>METRÓPOLE</t>
         </is>
       </c>
       <c r="V87" s="1">
-        <v>43805</v>
+        <v>42242</v>
       </c>
       <c r="W87" s="0">
         <v>0</v>
@@ -2973,34 +2938,19 @@
       </c>
       <c r="AB87" s="0" t="b">
         <v>0</v>
-      </c>
-      <c r="AC87" s="0" t="inlineStr">
-        <is>
-          <t>SANTANDER</t>
-        </is>
-      </c>
-      <c r="AD87" s="0" t="inlineStr">
-        <is>
-          <t>3201</t>
-        </is>
-      </c>
-      <c r="AE87" s="0" t="inlineStr">
-        <is>
-          <t>1005067-3</t>
-        </is>
       </c>
     </row>
     <row outlineLevel="0" r="88">
       <c r="A88" s="0">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="B88" s="0" t="inlineStr">
         <is>
-          <t>NBA</t>
+          <t>MOET HENNESSY</t>
         </is>
       </c>
       <c r="V88" s="1">
-        <v>43566</v>
+        <v>42446</v>
       </c>
       <c r="W88" s="0">
         <v>0</v>
@@ -3020,15 +2970,60 @@
     </row>
     <row outlineLevel="0" r="89">
       <c r="A89" s="0">
-        <v>153</v>
+        <v>99</v>
       </c>
       <c r="B89" s="0" t="inlineStr">
         <is>
-          <t>ND AMERICANAS</t>
+          <t>MOSTARDA PRODUÇÕES E EVENTOS LTDA - ME</t>
+        </is>
+      </c>
+      <c r="C89" s="0" t="inlineStr">
+        <is>
+          <t>MOSTARDA PRODUÇOES</t>
+        </is>
+      </c>
+      <c r="F89" s="0" t="inlineStr">
+        <is>
+          <t>RUA LEANDRO MARTINS, 10 SALA 902</t>
+        </is>
+      </c>
+      <c r="G89" s="0" t="inlineStr">
+        <is>
+          <t>CENTRO</t>
+        </is>
+      </c>
+      <c r="H89" s="0" t="inlineStr">
+        <is>
+          <t>RIO DE JANEIRO</t>
+        </is>
+      </c>
+      <c r="I89" s="0" t="inlineStr">
+        <is>
+          <t>RJ</t>
+        </is>
+      </c>
+      <c r="J89" s="0" t="inlineStr">
+        <is>
+          <t>20080-070</t>
+        </is>
+      </c>
+      <c r="L89" s="0" t="inlineStr">
+        <is>
+          <t>18.381.709/0001-40</t>
+        </is>
+      </c>
+      <c r="M89" s="0" t="inlineStr">
+        <is>
+          <t>ISENTO</t>
+        </is>
+      </c>
+      <c r="N89" s="0" t="inlineStr">
+        <is>
+          <t>0.582.179-7</t>
         </is>
       </c>
       <c r="V89" s="1">
-        <v>44419</v>
+        <v>43560</v>
       </c>
       <c r="W89" s="0">
         <v>0</v>
@@ -3048,15 +3043,20 @@
     </row>
     <row outlineLevel="0" r="90">
       <c r="A90" s="0">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B90" s="0" t="inlineStr">
         <is>
-          <t>NELIO/REGINA</t>
+          <t>NATHÁLIA QUINTANS</t>
+        </is>
+      </c>
+      <c r="O90" s="0" t="inlineStr">
+        <is>
+          <t>11010906771</t>
         </is>
       </c>
       <c r="V90" s="1">
-        <v>43802</v>
+        <v>43805</v>
       </c>
       <c r="W90" s="0">
         <v>0</v>
@@ -3071,20 +3071,35 @@
         <v>0</v>
       </c>
       <c r="AB90" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AC90" s="0" t="inlineStr">
+        <is>
+          <t>SANTANDER</t>
+        </is>
+      </c>
+      <c r="AD90" s="0" t="inlineStr">
+        <is>
+          <t>3201</t>
+        </is>
+      </c>
+      <c r="AE90" s="0" t="inlineStr">
+        <is>
+          <t>1005067-3</t>
+        </is>
       </c>
     </row>
     <row outlineLevel="0" r="91">
       <c r="A91" s="0">
-        <v>160</v>
+        <v>100</v>
       </c>
       <c r="B91" s="0" t="inlineStr">
         <is>
-          <t>NETZA</t>
+          <t>NBA</t>
         </is>
       </c>
       <c r="V91" s="1">
-        <v>44483</v>
+        <v>43566</v>
       </c>
       <c r="W91" s="0">
         <v>0</v>
@@ -3104,15 +3119,15 @@
     </row>
     <row outlineLevel="0" r="92">
       <c r="A92" s="0">
-        <v>8</v>
+        <v>153</v>
       </c>
       <c r="B92" s="0" t="inlineStr">
         <is>
-          <t>NIGHTRIO</t>
+          <t>ND AMERICANAS</t>
         </is>
       </c>
       <c r="V92" s="1">
-        <v>42149</v>
+        <v>44419</v>
       </c>
       <c r="W92" s="0">
         <v>0</v>
@@ -3132,15 +3147,15 @@
     </row>
     <row outlineLevel="0" r="93">
       <c r="A93" s="0">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="B93" s="0" t="inlineStr">
         <is>
-          <t>NORMAL PRA GENTE</t>
+          <t>NELIO/REGINA</t>
         </is>
       </c>
       <c r="V93" s="1">
-        <v>43524</v>
+        <v>43802</v>
       </c>
       <c r="W93" s="0">
         <v>0</v>
@@ -3155,20 +3170,20 @@
         <v>0</v>
       </c>
       <c r="AB93" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row outlineLevel="0" r="94">
       <c r="A94" s="0">
-        <v>90</v>
+        <v>160</v>
       </c>
       <c r="B94" s="0" t="inlineStr">
         <is>
-          <t>OLX</t>
+          <t>NETZA</t>
         </is>
       </c>
       <c r="V94" s="1">
-        <v>43326</v>
+        <v>44483</v>
       </c>
       <c r="W94" s="0">
         <v>0</v>
@@ -3188,15 +3203,15 @@
     </row>
     <row outlineLevel="0" r="95">
       <c r="A95" s="0">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="B95" s="0" t="inlineStr">
         <is>
-          <t>ORION BRANDING</t>
+          <t>NIGHTRIO</t>
         </is>
       </c>
       <c r="V95" s="1">
-        <v>42635</v>
+        <v>42149</v>
       </c>
       <c r="W95" s="0">
         <v>0</v>
@@ -3216,15 +3231,15 @@
     </row>
     <row outlineLevel="0" r="96">
       <c r="A96" s="0">
-        <v>136</v>
+        <v>97</v>
       </c>
       <c r="B96" s="0" t="inlineStr">
         <is>
-          <t>ORLA RIO</t>
+          <t>NORMAL PRA GENTE</t>
         </is>
       </c>
       <c r="V96" s="1">
-        <v>44161</v>
+        <v>43524</v>
       </c>
       <c r="W96" s="0">
         <v>0</v>
@@ -3244,25 +3259,15 @@
     </row>
     <row outlineLevel="0" r="97">
       <c r="A97" s="0">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="B97" s="0" t="inlineStr">
         <is>
-          <t>OS BATUTINHAS</t>
-        </is>
-      </c>
-      <c r="C97" s="0" t="inlineStr">
-        <is>
-          <t>OS BATUTINHAS ESPAÇO DE EDUC. INFANTIL LTDA</t>
-        </is>
-      </c>
-      <c r="L97" s="0" t="inlineStr">
-        <is>
-          <t>01.211.472/0001-56</t>
+          <t>OLX</t>
         </is>
       </c>
       <c r="V97" s="1">
-        <v>43651</v>
+        <v>43326</v>
       </c>
       <c r="W97" s="0">
         <v>0</v>
@@ -3282,15 +3287,15 @@
     </row>
     <row outlineLevel="0" r="98">
       <c r="A98" s="0">
-        <v>162</v>
+        <v>48</v>
       </c>
       <c r="B98" s="0" t="inlineStr">
         <is>
-          <t>OTALAB (CEREBRO)</t>
+          <t>ORION BRANDING</t>
         </is>
       </c>
       <c r="V98" s="1">
-        <v>44505</v>
+        <v>42635</v>
       </c>
       <c r="W98" s="0">
         <v>0</v>
@@ -3310,20 +3315,15 @@
     </row>
     <row outlineLevel="0" r="99">
       <c r="A99" s="0">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="B99" s="0" t="inlineStr">
         <is>
-          <t>ÓTIMA CONCESSIONÁRIA</t>
-        </is>
-      </c>
-      <c r="U99" s="0" t="inlineStr">
-        <is>
-          <t>anapaula.couto@otima.com</t>
+          <t>ORLA RIO</t>
         </is>
       </c>
       <c r="V99" s="1">
-        <v>44379</v>
+        <v>44161</v>
       </c>
       <c r="W99" s="0">
         <v>0</v>
@@ -3343,55 +3343,25 @@
     </row>
     <row outlineLevel="0" r="100">
       <c r="A100" s="0">
-        <v>147</v>
+        <v>108</v>
       </c>
       <c r="B100" s="0" t="inlineStr">
         <is>
-          <t>ÓTIMA CONCESSIONÁRIA DE EXPLORAÇÃO MOBILIÁRIO URBANO LTDA</t>
-        </is>
-      </c>
-      <c r="F100" s="0" t="inlineStr">
-        <is>
-          <t>RUA MOFARREJ, 1298</t>
-        </is>
-      </c>
-      <c r="G100" s="0" t="inlineStr">
-        <is>
-          <t>VILA LEOPOLDINA</t>
-        </is>
-      </c>
-      <c r="H100" s="0" t="inlineStr">
-        <is>
-          <t>SÃO PAULO</t>
-        </is>
-      </c>
-      <c r="I100" s="0" t="inlineStr">
-        <is>
-          <t>SP</t>
-        </is>
-      </c>
-      <c r="J100" s="0" t="inlineStr">
-        <is>
-          <t>06311-000</t>
+          <t>OS BATUTINHAS</t>
+        </is>
+      </c>
+      <c r="C100" s="0" t="inlineStr">
+        <is>
+          <t>OS BATUTINHAS ESPAÇO DE EDUC. INFANTIL LTDA</t>
         </is>
       </c>
       <c r="L100" s="0" t="inlineStr">
         <is>
-          <t>17.104.815/0001-13</t>
-        </is>
-      </c>
-      <c r="N100" s="0" t="inlineStr">
-        <is>
-          <t>4645058-0</t>
-        </is>
-      </c>
-      <c r="U100" s="0" t="inlineStr">
-        <is>
-          <t>anapaula.couto@otima.com (FINANCEIRO)</t>
+          <t>01.211.472/0001-56</t>
         </is>
       </c>
       <c r="V100" s="1">
-        <v>44347</v>
+        <v>43651</v>
       </c>
       <c r="W100" s="0">
         <v>0</v>
@@ -3411,15 +3381,15 @@
     </row>
     <row outlineLevel="0" r="101">
       <c r="A101" s="0">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="B101" s="0" t="inlineStr">
         <is>
-          <t>PAD BH</t>
+          <t>OTALAB (CEREBRO)</t>
         </is>
       </c>
       <c r="V101" s="1">
-        <v>44294</v>
+        <v>44505</v>
       </c>
       <c r="W101" s="0">
         <v>0</v>
@@ -3439,15 +3409,20 @@
     </row>
     <row outlineLevel="0" r="102">
       <c r="A102" s="0">
-        <v>39</v>
+        <v>149</v>
       </c>
       <c r="B102" s="0" t="inlineStr">
         <is>
-          <t>PAULO DE CASTRO</t>
+          <t>ÓTIMA CONCESSIONÁRIA</t>
+        </is>
+      </c>
+      <c r="U102" s="0" t="inlineStr">
+        <is>
+          <t>anapaula.couto@otima.com</t>
         </is>
       </c>
       <c r="V102" s="1">
-        <v>42471</v>
+        <v>44379</v>
       </c>
       <c r="W102" s="0">
         <v>0</v>
@@ -3467,15 +3442,55 @@
     </row>
     <row outlineLevel="0" r="103">
       <c r="A103" s="0">
-        <v>6</v>
+        <v>147</v>
       </c>
       <c r="B103" s="0" t="inlineStr">
         <is>
-          <t>PEDRO GUIMARÃES</t>
+          <t>ÓTIMA CONCESSIONÁRIA DE EXPLORAÇÃO MOBILIÁRIO URBANO LTDA</t>
+        </is>
+      </c>
+      <c r="F103" s="0" t="inlineStr">
+        <is>
+          <t>RUA MOFARREJ, 1298</t>
+        </is>
+      </c>
+      <c r="G103" s="0" t="inlineStr">
+        <is>
+          <t>VILA LEOPOLDINA</t>
+        </is>
+      </c>
+      <c r="H103" s="0" t="inlineStr">
+        <is>
+          <t>SÃO PAULO</t>
+        </is>
+      </c>
+      <c r="I103" s="0" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="J103" s="0" t="inlineStr">
+        <is>
+          <t>06311-000</t>
+        </is>
+      </c>
+      <c r="L103" s="0" t="inlineStr">
+        <is>
+          <t>17.104.815/0001-13</t>
+        </is>
+      </c>
+      <c r="N103" s="0" t="inlineStr">
+        <is>
+          <t>4645058-0</t>
+        </is>
+      </c>
+      <c r="U103" s="0" t="inlineStr">
+        <is>
+          <t>anapaula.couto@otima.com (FINANCEIRO)</t>
         </is>
       </c>
       <c r="V103" s="1">
-        <v>42136</v>
+        <v>44347</v>
       </c>
       <c r="W103" s="0">
         <v>0</v>
@@ -3495,15 +3510,15 @@
     </row>
     <row outlineLevel="0" r="104">
       <c r="A104" s="0">
-        <v>29</v>
+        <v>143</v>
       </c>
       <c r="B104" s="0" t="inlineStr">
         <is>
-          <t>PEDRO VILELA</t>
+          <t>PAD BH</t>
         </is>
       </c>
       <c r="V104" s="1">
-        <v>42359</v>
+        <v>44294</v>
       </c>
       <c r="W104" s="0">
         <v>0</v>
@@ -3523,15 +3538,15 @@
     </row>
     <row outlineLevel="0" r="105">
       <c r="A105" s="0">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B105" s="0" t="inlineStr">
         <is>
-          <t>Pernod Ricard</t>
+          <t>PAULO DE CASTRO</t>
         </is>
       </c>
       <c r="V105" s="1">
-        <v>42135</v>
+        <v>42471</v>
       </c>
       <c r="W105" s="0">
         <v>0</v>
@@ -3551,15 +3566,15 @@
     </row>
     <row outlineLevel="0" r="106">
       <c r="A106" s="0">
-        <v>126</v>
+        <v>6</v>
       </c>
       <c r="B106" s="0" t="inlineStr">
         <is>
-          <t>PLAY 9</t>
+          <t>PEDRO GUIMARÃES</t>
         </is>
       </c>
       <c r="V106" s="1">
-        <v>43846</v>
+        <v>42136</v>
       </c>
       <c r="W106" s="0">
         <v>0</v>
@@ -3579,15 +3594,15 @@
     </row>
     <row outlineLevel="0" r="107">
       <c r="A107" s="0">
-        <v>129</v>
+        <v>29</v>
       </c>
       <c r="B107" s="0" t="inlineStr">
         <is>
-          <t>PRODUTORA IDEIA REAL</t>
+          <t>PEDRO VILELA</t>
         </is>
       </c>
       <c r="V107" s="1">
-        <v>43900</v>
+        <v>42359</v>
       </c>
       <c r="W107" s="0">
         <v>0</v>
@@ -3607,15 +3622,15 @@
     </row>
     <row outlineLevel="0" r="108">
       <c r="A108" s="0">
-        <v>124</v>
+        <v>5</v>
       </c>
       <c r="B108" s="0" t="inlineStr">
         <is>
-          <t>REBECA KAIZER</t>
+          <t>Pernod Ricard</t>
         </is>
       </c>
       <c r="V108" s="1">
-        <v>43821</v>
+        <v>42135</v>
       </c>
       <c r="W108" s="0">
         <v>0</v>
@@ -3635,15 +3650,15 @@
     </row>
     <row outlineLevel="0" r="109">
       <c r="A109" s="0">
-        <v>43</v>
+        <v>126</v>
       </c>
       <c r="B109" s="0" t="inlineStr">
         <is>
-          <t>RED BULL</t>
+          <t>PLAY 9</t>
         </is>
       </c>
       <c r="V109" s="1">
-        <v>42511</v>
+        <v>43846</v>
       </c>
       <c r="W109" s="0">
         <v>0</v>
@@ -3663,15 +3678,15 @@
     </row>
     <row outlineLevel="0" r="110">
       <c r="A110" s="0">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B110" s="0" t="inlineStr">
         <is>
-          <t>RED DOOR</t>
+          <t>PRODUTORA IDEIA REAL</t>
         </is>
       </c>
       <c r="V110" s="1">
-        <v>44180</v>
+        <v>43900</v>
       </c>
       <c r="W110" s="0">
         <v>0</v>
@@ -3691,15 +3706,15 @@
     </row>
     <row outlineLevel="0" r="111">
       <c r="A111" s="0">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="B111" s="0" t="inlineStr">
         <is>
-          <t>RESERVA</t>
+          <t>REBECA KAIZER</t>
         </is>
       </c>
       <c r="V111" s="1">
-        <v>43154</v>
+        <v>43821</v>
       </c>
       <c r="W111" s="0">
         <v>0</v>
@@ -3719,15 +3734,15 @@
     </row>
     <row outlineLevel="0" r="112">
       <c r="A112" s="0">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="B112" s="0" t="inlineStr">
         <is>
-          <t>RIACHUELO IPANEMA</t>
+          <t>RED BULL</t>
         </is>
       </c>
       <c r="V112" s="1">
-        <v>42865</v>
+        <v>42511</v>
       </c>
       <c r="W112" s="0">
         <v>0</v>
@@ -3747,15 +3762,15 @@
     </row>
     <row outlineLevel="0" r="113">
       <c r="A113" s="0">
-        <v>79</v>
+        <v>137</v>
       </c>
       <c r="B113" s="0" t="inlineStr">
         <is>
-          <t>RIGGAR</t>
+          <t>RED DOOR</t>
         </is>
       </c>
       <c r="V113" s="1">
-        <v>43048</v>
+        <v>44180</v>
       </c>
       <c r="W113" s="0">
         <v>0</v>
@@ -3775,15 +3790,15 @@
     </row>
     <row outlineLevel="0" r="114">
       <c r="A114" s="0">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="B114" s="0" t="inlineStr">
         <is>
-          <t>RIOZOO</t>
+          <t>RESERVA</t>
         </is>
       </c>
       <c r="V114" s="1">
-        <v>43776</v>
+        <v>43154</v>
       </c>
       <c r="W114" s="0">
         <v>0</v>
@@ -3803,15 +3818,15 @@
     </row>
     <row outlineLevel="0" r="115">
       <c r="A115" s="0">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B115" s="0" t="inlineStr">
         <is>
-          <t>ROCK IN RIO</t>
+          <t>RIACHUELO IPANEMA</t>
         </is>
       </c>
       <c r="V115" s="1">
-        <v>42982</v>
+        <v>42865</v>
       </c>
       <c r="W115" s="0">
         <v>0</v>
@@ -3831,15 +3846,15 @@
     </row>
     <row outlineLevel="0" r="116">
       <c r="A116" s="0">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="B116" s="0" t="inlineStr">
         <is>
-          <t>RODRIGO LAMPREIA</t>
+          <t>RIGGAR</t>
         </is>
       </c>
       <c r="V116" s="1">
-        <v>42435</v>
+        <v>43048</v>
       </c>
       <c r="W116" s="0">
         <v>0</v>
@@ -3859,15 +3874,15 @@
     </row>
     <row outlineLevel="0" r="117">
       <c r="A117" s="0">
-        <v>22</v>
+        <v>117</v>
       </c>
       <c r="B117" s="0" t="inlineStr">
         <is>
-          <t>SCHEEEINS</t>
+          <t>RIOZOO</t>
         </is>
       </c>
       <c r="V117" s="1">
-        <v>42243</v>
+        <v>43776</v>
       </c>
       <c r="W117" s="0">
         <v>0</v>
@@ -3887,15 +3902,15 @@
     </row>
     <row outlineLevel="0" r="118">
       <c r="A118" s="0">
-        <v>127</v>
+        <v>74</v>
       </c>
       <c r="B118" s="0" t="inlineStr">
         <is>
-          <t>SCORE GROUP (SP)</t>
+          <t>ROCK IN RIO</t>
         </is>
       </c>
       <c r="V118" s="1">
-        <v>43852</v>
+        <v>42982</v>
       </c>
       <c r="W118" s="0">
         <v>0</v>
@@ -3915,15 +3930,15 @@
     </row>
     <row outlineLevel="0" r="119">
       <c r="A119" s="0">
-        <v>168</v>
+        <v>33</v>
       </c>
       <c r="B119" s="0" t="inlineStr">
         <is>
-          <t>SEBASTIAN</t>
+          <t>RODRIGO LAMPREIA</t>
         </is>
       </c>
       <c r="V119" s="1">
-        <v>44634</v>
+        <v>42435</v>
       </c>
       <c r="W119" s="0">
         <v>0</v>
@@ -3943,15 +3958,15 @@
     </row>
     <row outlineLevel="0" r="120">
       <c r="A120" s="0">
-        <v>150</v>
+        <v>22</v>
       </c>
       <c r="B120" s="0" t="inlineStr">
         <is>
-          <t>SEM EFEITO</t>
+          <t>SCHEEEINS</t>
         </is>
       </c>
       <c r="V120" s="1">
-        <v>44379</v>
+        <v>42243</v>
       </c>
       <c r="W120" s="0">
         <v>0</v>
@@ -3971,15 +3986,15 @@
     </row>
     <row outlineLevel="0" r="121">
       <c r="A121" s="0">
-        <v>68</v>
+        <v>127</v>
       </c>
       <c r="B121" s="0" t="inlineStr">
         <is>
-          <t>SEU VIDAL</t>
+          <t>SCORE GROUP (SP)</t>
         </is>
       </c>
       <c r="V121" s="1">
-        <v>42881</v>
+        <v>43852</v>
       </c>
       <c r="W121" s="0">
         <v>0</v>
@@ -3999,15 +4014,15 @@
     </row>
     <row outlineLevel="0" r="122">
       <c r="A122" s="0">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="B122" s="0" t="inlineStr">
         <is>
-          <t>SHERPA42</t>
+          <t>SEBASTIAN</t>
         </is>
       </c>
       <c r="V122" s="1">
-        <v>42677</v>
+        <v>44634</v>
       </c>
       <c r="W122" s="0">
         <v>0</v>
@@ -4027,15 +4042,15 @@
     </row>
     <row outlineLevel="0" r="123">
       <c r="A123" s="0">
-        <v>62</v>
+        <v>150</v>
       </c>
       <c r="B123" s="0" t="inlineStr">
         <is>
-          <t>SHOPPING BOULEVARD</t>
+          <t>SEM EFEITO</t>
         </is>
       </c>
       <c r="V123" s="1">
-        <v>42821</v>
+        <v>44379</v>
       </c>
       <c r="W123" s="0">
         <v>0</v>
@@ -4055,15 +4070,15 @@
     </row>
     <row outlineLevel="0" r="124">
       <c r="A124" s="0">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B124" s="0" t="inlineStr">
         <is>
-          <t>SHOPPING NOVA AMÉRICA</t>
+          <t>SEU VIDAL</t>
         </is>
       </c>
       <c r="V124" s="1">
-        <v>42863</v>
+        <v>42881</v>
       </c>
       <c r="W124" s="0">
         <v>0</v>
@@ -4083,20 +4098,15 @@
     </row>
     <row outlineLevel="0" r="125">
       <c r="A125" s="0">
-        <v>114</v>
+        <v>53</v>
       </c>
       <c r="B125" s="0" t="inlineStr">
         <is>
-          <t>SONHO DOS PÉS</t>
-        </is>
-      </c>
-      <c r="D125" s="0" t="inlineStr">
-        <is>
-          <t>Bárbara Soledade</t>
+          <t>SHERPA42</t>
         </is>
       </c>
       <c r="V125" s="1">
-        <v>43752</v>
+        <v>42677</v>
       </c>
       <c r="W125" s="0">
         <v>0</v>
@@ -4116,50 +4126,15 @@
     </row>
     <row outlineLevel="0" r="126">
       <c r="A126" s="0">
-        <v>133</v>
+        <v>62</v>
       </c>
       <c r="B126" s="0" t="inlineStr">
         <is>
-          <t>SORRIA</t>
-        </is>
-      </c>
-      <c r="C126" s="0" t="inlineStr">
-        <is>
-          <t>SORRIA</t>
-        </is>
-      </c>
-      <c r="F126" s="0" t="inlineStr">
-        <is>
-          <t>AV DAS HORTÊNCIAS,</t>
-        </is>
-      </c>
-      <c r="G126" s="0" t="inlineStr">
-        <is>
-          <t>AVENIDA CENTRAL</t>
-        </is>
-      </c>
-      <c r="H126" s="0" t="inlineStr">
-        <is>
-          <t>GRAMADO</t>
-        </is>
-      </c>
-      <c r="I126" s="0" t="inlineStr">
-        <is>
-          <t>RS</t>
-        </is>
-      </c>
-      <c r="J126" s="0" t="inlineStr">
-        <is>
-          <t>95670-000</t>
-        </is>
-      </c>
-      <c r="L126" s="0" t="inlineStr">
-        <is>
-          <t>34.573.787/0001-00</t>
+          <t>SHOPPING BOULEVARD</t>
         </is>
       </c>
       <c r="V126" s="1">
-        <v>44057</v>
+        <v>42821</v>
       </c>
       <c r="W126" s="0">
         <v>0</v>
@@ -4179,65 +4154,15 @@
     </row>
     <row outlineLevel="0" r="127">
       <c r="A127" s="0">
-        <v>164</v>
+        <v>65</v>
       </c>
       <c r="B127" s="0" t="inlineStr">
         <is>
-          <t>SPANTA NENEM</t>
-        </is>
-      </c>
-      <c r="C127" s="0" t="inlineStr">
-        <is>
-          <t>ASSOC E GR. RECR. BL CANAVALESCO SPANTA NENEM</t>
-        </is>
-      </c>
-      <c r="F127" s="0" t="inlineStr">
-        <is>
-          <t>RUA BARÃO DE LUCENA,32</t>
-        </is>
-      </c>
-      <c r="G127" s="0" t="inlineStr">
-        <is>
-          <t>BOTAFOGO</t>
-        </is>
-      </c>
-      <c r="H127" s="0" t="inlineStr">
-        <is>
-          <t>RIO DE JANEIRO</t>
-        </is>
-      </c>
-      <c r="I127" s="0" t="inlineStr">
-        <is>
-          <t>RJ</t>
-        </is>
-      </c>
-      <c r="J127" s="0" t="inlineStr">
-        <is>
-          <t>22260-020</t>
-        </is>
-      </c>
-      <c r="L127" s="0" t="inlineStr">
-        <is>
-          <t>07.094.273/0001-91</t>
-        </is>
-      </c>
-      <c r="M127" s="0" t="inlineStr">
-        <is>
-          <t>ISENTA</t>
-        </is>
-      </c>
-      <c r="N127" s="0" t="inlineStr">
-        <is>
-          <t>0497916-8</t>
-        </is>
-      </c>
-      <c r="Q127" s="0" t="inlineStr">
-        <is>
-          <t>21997276709</t>
+          <t>SHOPPING NOVA AMÉRICA</t>
         </is>
       </c>
       <c r="V127" s="1">
-        <v>44547</v>
+        <v>42863</v>
       </c>
       <c r="W127" s="0">
         <v>0</v>
@@ -4257,15 +4182,20 @@
     </row>
     <row outlineLevel="0" r="128">
       <c r="A128" s="0">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B128" s="0" t="inlineStr">
         <is>
-          <t>SPOLETO</t>
+          <t>SONHO DOS PÉS</t>
+        </is>
+      </c>
+      <c r="D128" s="0" t="inlineStr">
+        <is>
+          <t>Bárbara Soledade</t>
         </is>
       </c>
       <c r="V128" s="1">
-        <v>43766</v>
+        <v>43752</v>
       </c>
       <c r="W128" s="0">
         <v>0</v>
@@ -4285,15 +4215,50 @@
     </row>
     <row outlineLevel="0" r="129">
       <c r="A129" s="0">
-        <v>71</v>
+        <v>133</v>
       </c>
       <c r="B129" s="0" t="inlineStr">
         <is>
-          <t>SRCOM</t>
+          <t>SORRIA</t>
+        </is>
+      </c>
+      <c r="C129" s="0" t="inlineStr">
+        <is>
+          <t>SORRIA</t>
+        </is>
+      </c>
+      <c r="F129" s="0" t="inlineStr">
+        <is>
+          <t>AV DAS HORTÊNCIAS,</t>
+        </is>
+      </c>
+      <c r="G129" s="0" t="inlineStr">
+        <is>
+          <t>AVENIDA CENTRAL</t>
+        </is>
+      </c>
+      <c r="H129" s="0" t="inlineStr">
+        <is>
+          <t>GRAMADO</t>
+        </is>
+      </c>
+      <c r="I129" s="0" t="inlineStr">
+        <is>
+          <t>RS</t>
+        </is>
+      </c>
+      <c r="J129" s="0" t="inlineStr">
+        <is>
+          <t>95670-000</t>
+        </is>
+      </c>
+      <c r="L129" s="0" t="inlineStr">
+        <is>
+          <t>34.573.787/0001-00</t>
         </is>
       </c>
       <c r="V129" s="1">
-        <v>42926</v>
+        <v>44057</v>
       </c>
       <c r="W129" s="0">
         <v>0</v>
@@ -4313,15 +4278,65 @@
     </row>
     <row outlineLevel="0" r="130">
       <c r="A130" s="0">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="B130" s="0" t="inlineStr">
         <is>
-          <t>STAND EVE EMBAER</t>
+          <t>SPANTA NENEM</t>
+        </is>
+      </c>
+      <c r="C130" s="0" t="inlineStr">
+        <is>
+          <t>ASSOC E GR. RECR. BL CANAVALESCO SPANTA NENEM</t>
+        </is>
+      </c>
+      <c r="F130" s="0" t="inlineStr">
+        <is>
+          <t>RUA BARÃO DE LUCENA,32</t>
+        </is>
+      </c>
+      <c r="G130" s="0" t="inlineStr">
+        <is>
+          <t>BOTAFOGO</t>
+        </is>
+      </c>
+      <c r="H130" s="0" t="inlineStr">
+        <is>
+          <t>RIO DE JANEIRO</t>
+        </is>
+      </c>
+      <c r="I130" s="0" t="inlineStr">
+        <is>
+          <t>RJ</t>
+        </is>
+      </c>
+      <c r="J130" s="0" t="inlineStr">
+        <is>
+          <t>22260-020</t>
+        </is>
+      </c>
+      <c r="L130" s="0" t="inlineStr">
+        <is>
+          <t>07.094.273/0001-91</t>
+        </is>
+      </c>
+      <c r="M130" s="0" t="inlineStr">
+        <is>
+          <t>ISENTA</t>
+        </is>
+      </c>
+      <c r="N130" s="0" t="inlineStr">
+        <is>
+          <t>0497916-8</t>
+        </is>
+      </c>
+      <c r="Q130" s="0" t="inlineStr">
+        <is>
+          <t>21997276709</t>
         </is>
       </c>
       <c r="V130" s="1">
-        <v>44483</v>
+        <v>44547</v>
       </c>
       <c r="W130" s="0">
         <v>0</v>
@@ -4341,15 +4356,15 @@
     </row>
     <row outlineLevel="0" r="131">
       <c r="A131" s="0">
-        <v>7</v>
+        <v>115</v>
       </c>
       <c r="B131" s="0" t="inlineStr">
         <is>
-          <t>TAG</t>
+          <t>SPOLETO</t>
         </is>
       </c>
       <c r="V131" s="1">
-        <v>42149</v>
+        <v>43766</v>
       </c>
       <c r="W131" s="0">
         <v>0</v>
@@ -4369,15 +4384,15 @@
     </row>
     <row outlineLevel="0" r="132">
       <c r="A132" s="0">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="B132" s="0" t="inlineStr">
         <is>
-          <t>TAKE 4 CONTENT</t>
+          <t>SRCOM</t>
         </is>
       </c>
       <c r="V132" s="1">
-        <v>43375</v>
+        <v>42926</v>
       </c>
       <c r="W132" s="0">
         <v>0</v>
@@ -4397,15 +4412,15 @@
     </row>
     <row outlineLevel="0" r="133">
       <c r="A133" s="0">
-        <v>14</v>
+        <v>159</v>
       </c>
       <c r="B133" s="0" t="inlineStr">
         <is>
-          <t>TESTE</t>
+          <t>STAND EVE EMBAER</t>
         </is>
       </c>
       <c r="V133" s="1">
-        <v>42178</v>
+        <v>44483</v>
       </c>
       <c r="W133" s="0">
         <v>0</v>
@@ -4425,15 +4440,15 @@
     </row>
     <row outlineLevel="0" r="134">
       <c r="A134" s="0">
-        <v>111</v>
+        <v>7</v>
       </c>
       <c r="B134" s="0" t="inlineStr">
         <is>
-          <t>THIAGO P PACHECO</t>
+          <t>TAG</t>
         </is>
       </c>
       <c r="V134" s="1">
-        <v>43706</v>
+        <v>42149</v>
       </c>
       <c r="W134" s="0">
         <v>0</v>
@@ -4453,15 +4468,15 @@
     </row>
     <row outlineLevel="0" r="135">
       <c r="A135" s="0">
-        <v>145</v>
+        <v>92</v>
       </c>
       <c r="B135" s="0" t="inlineStr">
         <is>
-          <t>TWELVE MKT</t>
+          <t>TAKE 4 CONTENT</t>
         </is>
       </c>
       <c r="V135" s="1">
-        <v>44321</v>
+        <v>43375</v>
       </c>
       <c r="W135" s="0">
         <v>0</v>
@@ -4481,15 +4496,15 @@
     </row>
     <row outlineLevel="0" r="136">
       <c r="A136" s="0">
-        <v>139</v>
+        <v>14</v>
       </c>
       <c r="B136" s="0" t="inlineStr">
         <is>
-          <t>TWELVE SPORTS &amp; MARKETING LT</t>
+          <t>TESTE</t>
         </is>
       </c>
       <c r="V136" s="1">
-        <v>44231</v>
+        <v>42178</v>
       </c>
       <c r="W136" s="0">
         <v>0</v>
@@ -4509,15 +4524,15 @@
     </row>
     <row outlineLevel="0" r="137">
       <c r="A137" s="0">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="B137" s="0" t="inlineStr">
         <is>
-          <t>UEFA</t>
+          <t>THIAGO P PACHECO</t>
         </is>
       </c>
       <c r="V137" s="1">
-        <v>43539</v>
+        <v>43706</v>
       </c>
       <c r="W137" s="0">
         <v>0</v>
@@ -4537,15 +4552,15 @@
     </row>
     <row outlineLevel="0" r="138">
       <c r="A138" s="0">
-        <v>77</v>
+        <v>145</v>
       </c>
       <c r="B138" s="0" t="inlineStr">
         <is>
-          <t>UMA UMA</t>
+          <t>TWELVE MKT</t>
         </is>
       </c>
       <c r="V138" s="1">
-        <v>43011</v>
+        <v>44321</v>
       </c>
       <c r="W138" s="0">
         <v>0</v>
@@ -4565,15 +4580,15 @@
     </row>
     <row outlineLevel="0" r="139">
       <c r="A139" s="0">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B139" s="0" t="inlineStr">
         <is>
-          <t>UNLIMITED IDEIAS</t>
+          <t>TWELVE SPORTS &amp; MARKETING LT</t>
         </is>
       </c>
       <c r="V139" s="1">
-        <v>44250</v>
+        <v>44231</v>
       </c>
       <c r="W139" s="0">
         <v>0</v>
@@ -4593,15 +4608,15 @@
     </row>
     <row outlineLevel="0" r="140">
       <c r="A140" s="0">
-        <v>12</v>
+        <v>98</v>
       </c>
       <c r="B140" s="0" t="inlineStr">
         <is>
-          <t>UTILIZAR</t>
+          <t>UEFA</t>
         </is>
       </c>
       <c r="V140" s="1">
-        <v>42173</v>
+        <v>43539</v>
       </c>
       <c r="W140" s="0">
         <v>0</v>
@@ -4621,15 +4636,15 @@
     </row>
     <row outlineLevel="0" r="141">
       <c r="A141" s="0">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="B141" s="0" t="inlineStr">
         <is>
-          <t>VAL LASTRES</t>
+          <t>UMA UMA</t>
         </is>
       </c>
       <c r="V141" s="1">
-        <v>42271</v>
+        <v>43011</v>
       </c>
       <c r="W141" s="0">
         <v>0</v>
@@ -4649,15 +4664,15 @@
     </row>
     <row outlineLevel="0" r="142">
       <c r="A142" s="0">
-        <v>15</v>
+        <v>140</v>
       </c>
       <c r="B142" s="0" t="inlineStr">
         <is>
-          <t>VAMBORA</t>
+          <t>UNLIMITED IDEIAS</t>
         </is>
       </c>
       <c r="V142" s="1">
-        <v>42191</v>
+        <v>44250</v>
       </c>
       <c r="W142" s="0">
         <v>0</v>
@@ -4677,15 +4692,15 @@
     </row>
     <row outlineLevel="0" r="143">
       <c r="A143" s="0">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="B143" s="0" t="inlineStr">
         <is>
-          <t>VIBES &amp; TALZ</t>
+          <t>UTILIZAR</t>
         </is>
       </c>
       <c r="V143" s="1">
-        <v>43713</v>
+        <v>42173</v>
       </c>
       <c r="W143" s="0">
         <v>0</v>
@@ -4705,15 +4720,15 @@
     </row>
     <row outlineLevel="0" r="144">
       <c r="A144" s="0">
-        <v>73</v>
+        <v>169</v>
       </c>
       <c r="B144" s="0" t="inlineStr">
         <is>
-          <t>VICENTE DI GIORGIO</t>
+          <t>V3A</t>
         </is>
       </c>
       <c r="V144" s="1">
-        <v>42978</v>
+        <v>44645</v>
       </c>
       <c r="W144" s="0">
         <v>0</v>
@@ -4733,15 +4748,15 @@
     </row>
     <row outlineLevel="0" r="145">
       <c r="A145" s="0">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B145" s="0" t="inlineStr">
         <is>
-          <t>VILLAGE</t>
+          <t>VAL LASTRES</t>
         </is>
       </c>
       <c r="V145" s="1">
-        <v>42173</v>
+        <v>42271</v>
       </c>
       <c r="W145" s="0">
         <v>0</v>
@@ -4761,15 +4776,15 @@
     </row>
     <row outlineLevel="0" r="146">
       <c r="A146" s="0">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="B146" s="0" t="inlineStr">
         <is>
-          <t>VIRA</t>
+          <t>VAMBORA</t>
         </is>
       </c>
       <c r="V146" s="1">
-        <v>42859</v>
+        <v>42191</v>
       </c>
       <c r="W146" s="0">
         <v>0</v>
@@ -4789,15 +4804,15 @@
     </row>
     <row outlineLevel="0" r="147">
       <c r="A147" s="0">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="B147" s="0" t="inlineStr">
         <is>
-          <t>VIRA CENÁRIOS</t>
+          <t>VIBES &amp; TALZ</t>
         </is>
       </c>
       <c r="V147" s="1">
-        <v>43902</v>
+        <v>43713</v>
       </c>
       <c r="W147" s="0">
         <v>0</v>
@@ -4817,15 +4832,15 @@
     </row>
     <row outlineLevel="0" r="148">
       <c r="A148" s="0">
-        <v>154</v>
+        <v>73</v>
       </c>
       <c r="B148" s="0" t="inlineStr">
         <is>
-          <t>VIVO</t>
+          <t>VICENTE DI GIORGIO</t>
         </is>
       </c>
       <c r="V148" s="1">
-        <v>44446</v>
+        <v>42978</v>
       </c>
       <c r="W148" s="0">
         <v>0</v>
@@ -4845,15 +4860,15 @@
     </row>
     <row outlineLevel="0" r="149">
       <c r="A149" s="0">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B149" s="0" t="inlineStr">
         <is>
-          <t>VM-OFFICE</t>
+          <t>VILLAGE</t>
         </is>
       </c>
       <c r="V149" s="1">
-        <v>42485</v>
+        <v>42173</v>
       </c>
       <c r="W149" s="0">
         <v>0</v>
@@ -4873,15 +4888,15 @@
     </row>
     <row outlineLevel="0" r="150">
       <c r="A150" s="0">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="B150" s="0" t="inlineStr">
         <is>
-          <t>VODKA VOA</t>
+          <t>VIRA</t>
         </is>
       </c>
       <c r="V150" s="1">
-        <v>43507</v>
+        <v>42859</v>
       </c>
       <c r="W150" s="0">
         <v>0</v>
@@ -4901,15 +4916,15 @@
     </row>
     <row outlineLevel="0" r="151">
       <c r="A151" s="0">
-        <v>163</v>
+        <v>130</v>
       </c>
       <c r="B151" s="0" t="inlineStr">
         <is>
-          <t>VOE IDEIAS</t>
+          <t>VIRA CENÁRIOS</t>
         </is>
       </c>
       <c r="V151" s="1">
-        <v>44508</v>
+        <v>43902</v>
       </c>
       <c r="W151" s="0">
         <v>0</v>
@@ -4929,15 +4944,15 @@
     </row>
     <row outlineLevel="0" r="152">
       <c r="A152" s="0">
-        <v>42</v>
+        <v>154</v>
       </c>
       <c r="B152" s="0" t="inlineStr">
         <is>
-          <t>VOID</t>
+          <t>VIVO</t>
         </is>
       </c>
       <c r="V152" s="1">
-        <v>42501</v>
+        <v>44446</v>
       </c>
       <c r="W152" s="0">
         <v>0</v>
@@ -4957,15 +4972,15 @@
     </row>
     <row outlineLevel="0" r="153">
       <c r="A153" s="0">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="B153" s="0" t="inlineStr">
         <is>
-          <t>WGC</t>
+          <t>VM-OFFICE</t>
         </is>
       </c>
       <c r="V153" s="1">
-        <v>43060</v>
+        <v>42485</v>
       </c>
       <c r="W153" s="0">
         <v>0</v>
@@ -4985,15 +5000,15 @@
     </row>
     <row outlineLevel="0" r="154">
       <c r="A154" s="0">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="B154" s="0" t="inlineStr">
         <is>
-          <t>X3M - JUNIOR</t>
+          <t>VODKA VOA</t>
         </is>
       </c>
       <c r="V154" s="1">
-        <v>43706</v>
+        <v>43507</v>
       </c>
       <c r="W154" s="0">
         <v>0</v>
@@ -5013,29 +5028,141 @@
     </row>
     <row outlineLevel="0" r="155">
       <c r="A155" s="0">
+        <v>163</v>
+      </c>
+      <c r="B155" s="0" t="inlineStr">
+        <is>
+          <t>VOE IDEIAS</t>
+        </is>
+      </c>
+      <c r="V155" s="1">
+        <v>44508</v>
+      </c>
+      <c r="W155" s="0">
+        <v>0</v>
+      </c>
+      <c r="X155" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y155" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA155" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB155" s="0" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="156">
+      <c r="A156" s="0">
+        <v>42</v>
+      </c>
+      <c r="B156" s="0" t="inlineStr">
+        <is>
+          <t>VOID</t>
+        </is>
+      </c>
+      <c r="V156" s="1">
+        <v>42501</v>
+      </c>
+      <c r="W156" s="0">
+        <v>0</v>
+      </c>
+      <c r="X156" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y156" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA156" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB156" s="0" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="157">
+      <c r="A157" s="0">
+        <v>81</v>
+      </c>
+      <c r="B157" s="0" t="inlineStr">
+        <is>
+          <t>WGC</t>
+        </is>
+      </c>
+      <c r="V157" s="1">
+        <v>43060</v>
+      </c>
+      <c r="W157" s="0">
+        <v>0</v>
+      </c>
+      <c r="X157" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y157" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA157" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB157" s="0" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="158">
+      <c r="A158" s="0">
+        <v>110</v>
+      </c>
+      <c r="B158" s="0" t="inlineStr">
+        <is>
+          <t>X3M - JUNIOR</t>
+        </is>
+      </c>
+      <c r="V158" s="1">
+        <v>43706</v>
+      </c>
+      <c r="W158" s="0">
+        <v>0</v>
+      </c>
+      <c r="X158" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y158" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA158" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB158" s="0" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="159">
+      <c r="A159" s="0">
         <v>30</v>
       </c>
-      <c r="B155" s="0" t="inlineStr">
+      <c r="B159" s="0" t="inlineStr">
         <is>
           <t>ZEH PRETIM</t>
         </is>
       </c>
-      <c r="V155" s="1">
+      <c r="V159" s="1">
         <v>42391</v>
       </c>
-      <c r="W155" s="0">
-        <v>0</v>
-      </c>
-      <c r="X155" s="0">
-        <v>0</v>
-      </c>
-      <c r="Y155" s="0">
-        <v>0</v>
-      </c>
-      <c r="AA155" s="0">
-        <v>0</v>
-      </c>
-      <c r="AB155" s="0" t="b">
+      <c r="W159" s="0">
+        <v>0</v>
+      </c>
+      <c r="X159" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y159" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA159" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB159" s="0" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adiciona favicon e melhora performance no kendogrid
</commit_message>
<xml_diff>
--- a/public/migracao/clientes1.xlsx
+++ b/public/migracao/clientes1.xlsx
@@ -10,7 +10,7 @@
     <sheet sheetId="1" r:id="rId1" name="Clientes"/>
   </sheets>
   <definedNames>
-    <definedName name="Clientes">'Clientes'!$A$1:$AE$159</definedName>
+    <definedName name="Clientes">'Clientes'!$A$1:$AE$160</definedName>
   </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
@@ -347,7 +347,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE159"/>
+  <dimension ref="A1:AE160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -939,15 +939,15 @@
     </row>
     <row outlineLevel="0" r="17">
       <c r="A17" s="0">
-        <v>54</v>
+        <v>174</v>
       </c>
       <c r="B17" s="0" t="inlineStr">
         <is>
-          <t>BRASA FOODIES</t>
+          <t>BETTER DRINKS</t>
         </is>
       </c>
       <c r="V17" s="1">
-        <v>42677</v>
+        <v>44700</v>
       </c>
       <c r="W17" s="0">
         <v>0</v>
@@ -967,15 +967,15 @@
     </row>
     <row outlineLevel="0" r="18">
       <c r="A18" s="0">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B18" s="0" t="inlineStr">
         <is>
-          <t>BRMALLS</t>
+          <t>BRASA FOODIES</t>
         </is>
       </c>
       <c r="V18" s="1">
-        <v>42545</v>
+        <v>42677</v>
       </c>
       <c r="W18" s="0">
         <v>0</v>
@@ -995,15 +995,15 @@
     </row>
     <row outlineLevel="0" r="19">
       <c r="A19" s="0">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B19" s="0" t="inlineStr">
         <is>
-          <t>BRUNO BEZERRA</t>
+          <t>BRMALLS</t>
         </is>
       </c>
       <c r="V19" s="1">
-        <v>42446</v>
+        <v>42545</v>
       </c>
       <c r="W19" s="0">
         <v>0</v>
@@ -1023,15 +1023,15 @@
     </row>
     <row outlineLevel="0" r="20">
       <c r="A20" s="0">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B20" s="0" t="inlineStr">
         <is>
-          <t>BRUNO LANDEIRA</t>
+          <t>BRUNO BEZERRA</t>
         </is>
       </c>
       <c r="V20" s="1">
-        <v>42241</v>
+        <v>42446</v>
       </c>
       <c r="W20" s="0">
         <v>0</v>
@@ -1051,15 +1051,15 @@
     </row>
     <row outlineLevel="0" r="21">
       <c r="A21" s="0">
-        <v>123</v>
+        <v>20</v>
       </c>
       <c r="B21" s="0" t="inlineStr">
         <is>
-          <t>BRUNO MEROLLA</t>
+          <t>BRUNO LANDEIRA</t>
         </is>
       </c>
       <c r="V21" s="1">
-        <v>43819</v>
+        <v>42241</v>
       </c>
       <c r="W21" s="0">
         <v>0</v>
@@ -1079,15 +1079,15 @@
     </row>
     <row outlineLevel="0" r="22">
       <c r="A22" s="0">
-        <v>158</v>
+        <v>123</v>
       </c>
       <c r="B22" s="0" t="inlineStr">
         <is>
-          <t>CACO DE VIDRO</t>
+          <t>BRUNO MEROLLA</t>
         </is>
       </c>
       <c r="V22" s="1">
-        <v>44475</v>
+        <v>43819</v>
       </c>
       <c r="W22" s="0">
         <v>0</v>
@@ -1107,15 +1107,15 @@
     </row>
     <row outlineLevel="0" r="23">
       <c r="A23" s="0">
-        <v>83</v>
+        <v>158</v>
       </c>
       <c r="B23" s="0" t="inlineStr">
         <is>
-          <t>CAMAROTE ALEGRIA 2018</t>
+          <t>CACO DE VIDRO</t>
         </is>
       </c>
       <c r="V23" s="1">
-        <v>43122</v>
+        <v>44475</v>
       </c>
       <c r="W23" s="0">
         <v>0</v>
@@ -1135,15 +1135,15 @@
     </row>
     <row outlineLevel="0" r="24">
       <c r="A24" s="0">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="B24" s="0" t="inlineStr">
         <is>
-          <t>CAMAROTE RIO</t>
+          <t>CAMAROTE ALEGRIA 2018</t>
         </is>
       </c>
       <c r="V24" s="1">
-        <v>43522</v>
+        <v>43122</v>
       </c>
       <c r="W24" s="0">
         <v>0</v>
@@ -1163,15 +1163,15 @@
     </row>
     <row outlineLevel="0" r="25">
       <c r="A25" s="0">
-        <v>26</v>
+        <v>96</v>
       </c>
       <c r="B25" s="0" t="inlineStr">
         <is>
-          <t>CANAL OFF</t>
+          <t>CAMAROTE RIO</t>
         </is>
       </c>
       <c r="V25" s="1">
-        <v>42337</v>
+        <v>43522</v>
       </c>
       <c r="W25" s="0">
         <v>0</v>
@@ -1191,15 +1191,15 @@
     </row>
     <row outlineLevel="0" r="26">
       <c r="A26" s="0">
-        <v>144</v>
+        <v>26</v>
       </c>
       <c r="B26" s="0" t="inlineStr">
         <is>
-          <t>CASTAS</t>
+          <t>CANAL OFF</t>
         </is>
       </c>
       <c r="V26" s="1">
-        <v>44314</v>
+        <v>42337</v>
       </c>
       <c r="W26" s="0">
         <v>0</v>
@@ -1219,15 +1219,15 @@
     </row>
     <row outlineLevel="0" r="27">
       <c r="A27" s="0">
-        <v>31</v>
+        <v>144</v>
       </c>
       <c r="B27" s="0" t="inlineStr">
         <is>
-          <t>CB PRODUÇÕES</t>
+          <t>CASTAS</t>
         </is>
       </c>
       <c r="V27" s="1">
-        <v>42432</v>
+        <v>44314</v>
       </c>
       <c r="W27" s="0">
         <v>0</v>
@@ -1247,15 +1247,15 @@
     </row>
     <row outlineLevel="0" r="28">
       <c r="A28" s="0">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="B28" s="0" t="inlineStr">
         <is>
-          <t>CERVEJARIA  PRAYA</t>
+          <t>CB PRODUÇÕES</t>
         </is>
       </c>
       <c r="V28" s="1">
-        <v>42621</v>
+        <v>42432</v>
       </c>
       <c r="W28" s="0">
         <v>0</v>
@@ -1275,15 +1275,15 @@
     </row>
     <row outlineLevel="0" r="29">
       <c r="A29" s="0">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B29" s="0" t="inlineStr">
         <is>
-          <t>CERVEJARIA PRAYA</t>
+          <t>CERVEJARIA  PRAYA</t>
         </is>
       </c>
       <c r="V29" s="1">
-        <v>42523</v>
+        <v>42621</v>
       </c>
       <c r="W29" s="0">
         <v>0</v>
@@ -1303,15 +1303,15 @@
     </row>
     <row outlineLevel="0" r="30">
       <c r="A30" s="0">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="B30" s="0" t="inlineStr">
         <is>
-          <t>CERVEJARIA TEREZÓPOLIS</t>
+          <t>CERVEJARIA PRAYA</t>
         </is>
       </c>
       <c r="V30" s="1">
-        <v>42881</v>
+        <v>42523</v>
       </c>
       <c r="W30" s="0">
         <v>0</v>
@@ -1331,15 +1331,15 @@
     </row>
     <row outlineLevel="0" r="31">
       <c r="A31" s="0">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B31" s="0" t="inlineStr">
         <is>
-          <t>CHIQUINHO - TOTO</t>
+          <t>CERVEJARIA TEREZÓPOLIS</t>
         </is>
       </c>
       <c r="V31" s="1">
-        <v>42956</v>
+        <v>42881</v>
       </c>
       <c r="W31" s="0">
         <v>0</v>
@@ -1359,15 +1359,15 @@
     </row>
     <row outlineLevel="0" r="32">
       <c r="A32" s="0">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B32" s="0" t="inlineStr">
         <is>
-          <t>CIA MULLER DE BEBIDAS</t>
+          <t>CHIQUINHO - TOTO</t>
         </is>
       </c>
       <c r="V32" s="1">
-        <v>42992</v>
+        <v>42956</v>
       </c>
       <c r="W32" s="0">
         <v>0</v>
@@ -1387,15 +1387,15 @@
     </row>
     <row outlineLevel="0" r="33">
       <c r="A33" s="0">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="B33" s="0" t="inlineStr">
         <is>
-          <t>CLEAR CHANNEL</t>
+          <t>CIA MULLER DE BEBIDAS</t>
         </is>
       </c>
       <c r="V33" s="1">
-        <v>42554</v>
+        <v>42992</v>
       </c>
       <c r="W33" s="0">
         <v>0</v>
@@ -1415,15 +1415,15 @@
     </row>
     <row outlineLevel="0" r="34">
       <c r="A34" s="0">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B34" s="0" t="inlineStr">
         <is>
-          <t>COOL PRODUÇÕES</t>
+          <t>CLEAR CHANNEL</t>
         </is>
       </c>
       <c r="V34" s="1">
-        <v>42466</v>
+        <v>42554</v>
       </c>
       <c r="W34" s="0">
         <v>0</v>
@@ -1443,15 +1443,15 @@
     </row>
     <row outlineLevel="0" r="35">
       <c r="A35" s="0">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B35" s="0" t="inlineStr">
         <is>
-          <t>CRIAATVA</t>
+          <t>COOL PRODUÇÕES</t>
         </is>
       </c>
       <c r="V35" s="1">
-        <v>42171</v>
+        <v>42466</v>
       </c>
       <c r="W35" s="0">
         <v>0</v>
@@ -1471,15 +1471,15 @@
     </row>
     <row outlineLevel="0" r="36">
       <c r="A36" s="0">
-        <v>91</v>
+        <v>11</v>
       </c>
       <c r="B36" s="0" t="inlineStr">
         <is>
-          <t>CS EVENTOS</t>
+          <t>CRIAATVA</t>
         </is>
       </c>
       <c r="V36" s="1">
-        <v>43354</v>
+        <v>42171</v>
       </c>
       <c r="W36" s="0">
         <v>0</v>
@@ -1499,15 +1499,15 @@
     </row>
     <row outlineLevel="0" r="37">
       <c r="A37" s="0">
-        <v>152</v>
+        <v>91</v>
       </c>
       <c r="B37" s="0" t="inlineStr">
         <is>
-          <t>D2S SERVIÇO DE SEGURANÇA</t>
+          <t>CS EVENTOS</t>
         </is>
       </c>
       <c r="V37" s="1">
-        <v>44405</v>
+        <v>43354</v>
       </c>
       <c r="W37" s="0">
         <v>0</v>
@@ -1527,15 +1527,15 @@
     </row>
     <row outlineLevel="0" r="38">
       <c r="A38" s="0">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B38" s="0" t="inlineStr">
         <is>
-          <t>DANI SOLON</t>
+          <t>D2S SERVIÇO DE SEGURANÇA</t>
         </is>
       </c>
       <c r="V38" s="1">
-        <v>44447</v>
+        <v>44405</v>
       </c>
       <c r="W38" s="0">
         <v>0</v>
@@ -1555,15 +1555,15 @@
     </row>
     <row outlineLevel="0" r="39">
       <c r="A39" s="0">
-        <v>61</v>
+        <v>155</v>
       </c>
       <c r="B39" s="0" t="inlineStr">
         <is>
-          <t>DELETADA</t>
+          <t>DANI SOLON</t>
         </is>
       </c>
       <c r="V39" s="1">
-        <v>42802</v>
+        <v>44447</v>
       </c>
       <c r="W39" s="0">
         <v>0</v>
@@ -1583,15 +1583,15 @@
     </row>
     <row outlineLevel="0" r="40">
       <c r="A40" s="0">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B40" s="0" t="inlineStr">
         <is>
-          <t>DIAGEO</t>
+          <t>DELETADA</t>
         </is>
       </c>
       <c r="V40" s="1">
-        <v>43007</v>
+        <v>42802</v>
       </c>
       <c r="W40" s="0">
         <v>0</v>
@@ -1611,15 +1611,15 @@
     </row>
     <row outlineLevel="0" r="41">
       <c r="A41" s="0">
-        <v>156</v>
+        <v>76</v>
       </c>
       <c r="B41" s="0" t="inlineStr">
         <is>
-          <t>DIALOGO URBANO - BARBARA SOLEDADE</t>
+          <t>DIAGEO</t>
         </is>
       </c>
       <c r="V41" s="1">
-        <v>44448</v>
+        <v>43007</v>
       </c>
       <c r="W41" s="0">
         <v>0</v>
@@ -1639,15 +1639,15 @@
     </row>
     <row outlineLevel="0" r="42">
       <c r="A42" s="0">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B42" s="0" t="inlineStr">
         <is>
-          <t>DION ME</t>
+          <t>DIALOGO URBANO - BARBARA SOLEDADE</t>
         </is>
       </c>
       <c r="V42" s="1">
-        <v>44452</v>
+        <v>44448</v>
       </c>
       <c r="W42" s="0">
         <v>0</v>
@@ -1667,15 +1667,15 @@
     </row>
     <row outlineLevel="0" r="43">
       <c r="A43" s="0">
-        <v>63</v>
+        <v>157</v>
       </c>
       <c r="B43" s="0" t="inlineStr">
         <is>
-          <t>DOMINUS - BRAMEX</t>
+          <t>DION ME</t>
         </is>
       </c>
       <c r="V43" s="1">
-        <v>42831</v>
+        <v>44452</v>
       </c>
       <c r="W43" s="0">
         <v>0</v>
@@ -1695,15 +1695,15 @@
     </row>
     <row outlineLevel="0" r="44">
       <c r="A44" s="0">
-        <v>105</v>
+        <v>63</v>
       </c>
       <c r="B44" s="0" t="inlineStr">
         <is>
-          <t>DREAM FACTORY</t>
+          <t>DOMINUS - BRAMEX</t>
         </is>
       </c>
       <c r="V44" s="1">
-        <v>43633</v>
+        <v>42831</v>
       </c>
       <c r="W44" s="0">
         <v>0</v>
@@ -1723,15 +1723,15 @@
     </row>
     <row outlineLevel="0" r="45">
       <c r="A45" s="0">
-        <v>17</v>
+        <v>105</v>
       </c>
       <c r="B45" s="0" t="inlineStr">
         <is>
-          <t>DUDA GASPAR</t>
+          <t>DREAM FACTORY</t>
         </is>
       </c>
       <c r="V45" s="1">
-        <v>42200</v>
+        <v>43633</v>
       </c>
       <c r="W45" s="0">
         <v>0</v>
@@ -1751,15 +1751,15 @@
     </row>
     <row outlineLevel="0" r="46">
       <c r="A46" s="0">
-        <v>101</v>
+        <v>17</v>
       </c>
       <c r="B46" s="0" t="inlineStr">
         <is>
-          <t>ELEMENTAL 5</t>
+          <t>DUDA GASPAR</t>
         </is>
       </c>
       <c r="V46" s="1">
-        <v>43579</v>
+        <v>42200</v>
       </c>
       <c r="W46" s="0">
         <v>0</v>
@@ -1779,15 +1779,15 @@
     </row>
     <row outlineLevel="0" r="47">
       <c r="A47" s="0">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="B47" s="0" t="inlineStr">
         <is>
-          <t>ESCOLA ELEVA</t>
+          <t>ELEMENTAL 5</t>
         </is>
       </c>
       <c r="V47" s="1">
-        <v>42885</v>
+        <v>43579</v>
       </c>
       <c r="W47" s="0">
         <v>0</v>
@@ -1807,15 +1807,15 @@
     </row>
     <row outlineLevel="0" r="48">
       <c r="A48" s="0">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="B48" s="0" t="inlineStr">
         <is>
-          <t>FÁBRICA</t>
+          <t>ESCOLA ELEVA</t>
         </is>
       </c>
       <c r="V48" s="1">
-        <v>43805</v>
+        <v>42885</v>
       </c>
       <c r="W48" s="0">
         <v>0</v>
@@ -1835,15 +1835,15 @@
     </row>
     <row outlineLevel="0" r="49">
       <c r="A49" s="0">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="B49" s="0" t="inlineStr">
         <is>
-          <t>FÁBRICA.AG</t>
+          <t>FÁBRICA</t>
         </is>
       </c>
       <c r="V49" s="1">
-        <v>44280</v>
+        <v>43805</v>
       </c>
       <c r="W49" s="0">
         <v>0</v>
@@ -1863,15 +1863,15 @@
     </row>
     <row outlineLevel="0" r="50">
       <c r="A50" s="0">
-        <v>87</v>
+        <v>142</v>
       </c>
       <c r="B50" s="0" t="inlineStr">
         <is>
-          <t>FABRÍCIO STOFEL</t>
+          <t>FÁBRICA.AG</t>
         </is>
       </c>
       <c r="V50" s="1">
-        <v>43248</v>
+        <v>44280</v>
       </c>
       <c r="W50" s="0">
         <v>0</v>
@@ -1891,15 +1891,15 @@
     </row>
     <row outlineLevel="0" r="51">
       <c r="A51" s="0">
-        <v>135</v>
+        <v>87</v>
       </c>
       <c r="B51" s="0" t="inlineStr">
         <is>
-          <t>FAIRMONT</t>
+          <t>FABRÍCIO STOFEL</t>
         </is>
       </c>
       <c r="V51" s="1">
-        <v>44161</v>
+        <v>43248</v>
       </c>
       <c r="W51" s="0">
         <v>0</v>
@@ -1919,15 +1919,15 @@
     </row>
     <row outlineLevel="0" r="52">
       <c r="A52" s="0">
-        <v>58</v>
+        <v>135</v>
       </c>
       <c r="B52" s="0" t="inlineStr">
         <is>
-          <t>FARM</t>
+          <t>FAIRMONT</t>
         </is>
       </c>
       <c r="V52" s="1">
-        <v>42754</v>
+        <v>44161</v>
       </c>
       <c r="W52" s="0">
         <v>0</v>
@@ -1947,15 +1947,15 @@
     </row>
     <row outlineLevel="0" r="53">
       <c r="A53" s="0">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="B53" s="0" t="inlineStr">
         <is>
-          <t>FELIPE BITTENCOURT</t>
+          <t>FARM</t>
         </is>
       </c>
       <c r="V53" s="1">
-        <v>43520</v>
+        <v>42754</v>
       </c>
       <c r="W53" s="0">
         <v>0</v>
@@ -1975,15 +1975,15 @@
     </row>
     <row outlineLevel="0" r="54">
       <c r="A54" s="0">
-        <v>161</v>
+        <v>95</v>
       </c>
       <c r="B54" s="0" t="inlineStr">
         <is>
-          <t>FLYSPORTS</t>
+          <t>FELIPE BITTENCOURT</t>
         </is>
       </c>
       <c r="V54" s="1">
-        <v>44483</v>
+        <v>43520</v>
       </c>
       <c r="W54" s="0">
         <v>0</v>
@@ -2003,15 +2003,15 @@
     </row>
     <row outlineLevel="0" r="55">
       <c r="A55" s="0">
-        <v>40</v>
+        <v>161</v>
       </c>
       <c r="B55" s="0" t="inlineStr">
         <is>
-          <t>FOODIES</t>
+          <t>FLYSPORTS</t>
         </is>
       </c>
       <c r="V55" s="1">
-        <v>42475</v>
+        <v>44483</v>
       </c>
       <c r="W55" s="0">
         <v>0</v>
@@ -2031,15 +2031,15 @@
     </row>
     <row outlineLevel="0" r="56">
       <c r="A56" s="0">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B56" s="0" t="inlineStr">
         <is>
-          <t>FOXTON</t>
+          <t>FOODIES</t>
         </is>
       </c>
       <c r="V56" s="1">
-        <v>42649</v>
+        <v>42475</v>
       </c>
       <c r="W56" s="0">
         <v>0</v>
@@ -2059,15 +2059,15 @@
     </row>
     <row outlineLevel="0" r="57">
       <c r="A57" s="0">
-        <v>148</v>
+        <v>50</v>
       </c>
       <c r="B57" s="0" t="inlineStr">
         <is>
-          <t>GENEAL</t>
+          <t>FOXTON</t>
         </is>
       </c>
       <c r="V57" s="1">
-        <v>44363</v>
+        <v>42649</v>
       </c>
       <c r="W57" s="0">
         <v>0</v>
@@ -2087,30 +2087,15 @@
     </row>
     <row outlineLevel="0" r="58">
       <c r="A58" s="0">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="B58" s="0" t="inlineStr">
         <is>
-          <t>GLOBO COMUNICAÇÕES</t>
-        </is>
-      </c>
-      <c r="F58" s="0" t="inlineStr">
-        <is>
-          <t>RUA LOPES QUINTTAS, 303</t>
-        </is>
-      </c>
-      <c r="G58" s="0" t="inlineStr">
-        <is>
-          <t>JARDIM BOTANICO</t>
-        </is>
-      </c>
-      <c r="L58" s="0" t="inlineStr">
-        <is>
-          <t>27.865.757/0001-02</t>
+          <t>GENEAL</t>
         </is>
       </c>
       <c r="V58" s="1">
-        <v>44669</v>
+        <v>44363</v>
       </c>
       <c r="W58" s="0">
         <v>0</v>
@@ -2130,15 +2115,30 @@
     </row>
     <row outlineLevel="0" r="59">
       <c r="A59" s="0">
-        <v>51</v>
+        <v>171</v>
       </c>
       <c r="B59" s="0" t="inlineStr">
         <is>
-          <t>GLOBO SAT</t>
+          <t>GLOBO COMUNICAÇÕES</t>
+        </is>
+      </c>
+      <c r="F59" s="0" t="inlineStr">
+        <is>
+          <t>RUA LOPES QUINTTAS, 303</t>
+        </is>
+      </c>
+      <c r="G59" s="0" t="inlineStr">
+        <is>
+          <t>JARDIM BOTANICO</t>
+        </is>
+      </c>
+      <c r="L59" s="0" t="inlineStr">
+        <is>
+          <t>27.865.757/0001-02</t>
         </is>
       </c>
       <c r="V59" s="1">
-        <v>42656</v>
+        <v>44669</v>
       </c>
       <c r="W59" s="0">
         <v>0</v>
@@ -2158,15 +2158,15 @@
     </row>
     <row outlineLevel="0" r="60">
       <c r="A60" s="0">
-        <v>121</v>
+        <v>51</v>
       </c>
       <c r="B60" s="0" t="inlineStr">
         <is>
-          <t>GLOBOPLAY</t>
+          <t>GLOBO SAT</t>
         </is>
       </c>
       <c r="V60" s="1">
-        <v>43817</v>
+        <v>42656</v>
       </c>
       <c r="W60" s="0">
         <v>0</v>
@@ -2186,15 +2186,15 @@
     </row>
     <row outlineLevel="0" r="61">
       <c r="A61" s="0">
-        <v>25</v>
+        <v>121</v>
       </c>
       <c r="B61" s="0" t="inlineStr">
         <is>
-          <t>GMP</t>
+          <t>GLOBOPLAY</t>
         </is>
       </c>
       <c r="V61" s="1">
-        <v>42334</v>
+        <v>43817</v>
       </c>
       <c r="W61" s="0">
         <v>0</v>
@@ -2214,15 +2214,15 @@
     </row>
     <row outlineLevel="0" r="62">
       <c r="A62" s="0">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B62" s="0" t="inlineStr">
         <is>
-          <t>GRUPO 8</t>
+          <t>GMP</t>
         </is>
       </c>
       <c r="V62" s="1">
-        <v>42453</v>
+        <v>42334</v>
       </c>
       <c r="W62" s="0">
         <v>0</v>
@@ -2242,15 +2242,15 @@
     </row>
     <row outlineLevel="0" r="63">
       <c r="A63" s="0">
-        <v>104</v>
+        <v>37</v>
       </c>
       <c r="B63" s="0" t="inlineStr">
         <is>
-          <t>GRUPO CATARATAS</t>
+          <t>GRUPO 8</t>
         </is>
       </c>
       <c r="V63" s="1">
-        <v>43596</v>
+        <v>42453</v>
       </c>
       <c r="W63" s="0">
         <v>0</v>
@@ -2270,15 +2270,15 @@
     </row>
     <row outlineLevel="0" r="64">
       <c r="A64" s="0">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="B64" s="0" t="inlineStr">
         <is>
-          <t>HANDRED</t>
+          <t>GRUPO CATARATAS</t>
         </is>
       </c>
       <c r="V64" s="1">
-        <v>42872</v>
+        <v>43596</v>
       </c>
       <c r="W64" s="0">
         <v>0</v>
@@ -2298,15 +2298,15 @@
     </row>
     <row outlineLevel="0" r="65">
       <c r="A65" s="0">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="B65" s="0" t="inlineStr">
         <is>
-          <t>HARRISON</t>
+          <t>HANDRED</t>
         </is>
       </c>
       <c r="V65" s="1">
-        <v>42165</v>
+        <v>42872</v>
       </c>
       <c r="W65" s="0">
         <v>0</v>
@@ -2326,15 +2326,15 @@
     </row>
     <row outlineLevel="0" r="66">
       <c r="A66" s="0">
-        <v>113</v>
+        <v>9</v>
       </c>
       <c r="B66" s="0" t="inlineStr">
         <is>
-          <t>HAUTE</t>
+          <t>HARRISON</t>
         </is>
       </c>
       <c r="V66" s="1">
-        <v>43720</v>
+        <v>42165</v>
       </c>
       <c r="W66" s="0">
         <v>0</v>
@@ -2354,15 +2354,15 @@
     </row>
     <row outlineLevel="0" r="67">
       <c r="A67" s="0">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="B67" s="0" t="inlineStr">
         <is>
-          <t>HEADS</t>
+          <t>HAUTE</t>
         </is>
       </c>
       <c r="V67" s="1">
-        <v>43399</v>
+        <v>43720</v>
       </c>
       <c r="W67" s="0">
         <v>0</v>
@@ -2382,15 +2382,15 @@
     </row>
     <row outlineLevel="0" r="68">
       <c r="A68" s="0">
-        <v>4</v>
+        <v>93</v>
       </c>
       <c r="B68" s="0" t="inlineStr">
         <is>
-          <t>HEINEKEN</t>
+          <t>HEADS</t>
         </is>
       </c>
       <c r="V68" s="1">
-        <v>42133</v>
+        <v>43399</v>
       </c>
       <c r="W68" s="0">
         <v>0</v>
@@ -2410,15 +2410,15 @@
     </row>
     <row outlineLevel="0" r="69">
       <c r="A69" s="0">
-        <v>86</v>
+        <v>4</v>
       </c>
       <c r="B69" s="0" t="inlineStr">
         <is>
-          <t>HUB BRASIL</t>
+          <t>HEINEKEN</t>
         </is>
       </c>
       <c r="V69" s="1">
-        <v>43238</v>
+        <v>42133</v>
       </c>
       <c r="W69" s="0">
         <v>0</v>
@@ -2438,15 +2438,15 @@
     </row>
     <row outlineLevel="0" r="70">
       <c r="A70" s="0">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="B70" s="0" t="inlineStr">
         <is>
-          <t>HUG ENTRETERIMENTO</t>
+          <t>HUB BRASIL</t>
         </is>
       </c>
       <c r="V70" s="1">
-        <v>42780</v>
+        <v>43238</v>
       </c>
       <c r="W70" s="0">
         <v>0</v>
@@ -2466,15 +2466,15 @@
     </row>
     <row outlineLevel="0" r="71">
       <c r="A71" s="0">
-        <v>131</v>
+        <v>60</v>
       </c>
       <c r="B71" s="0" t="inlineStr">
         <is>
-          <t>IABAS</t>
+          <t>HUG ENTRETERIMENTO</t>
         </is>
       </c>
       <c r="V71" s="1">
-        <v>43937</v>
+        <v>42780</v>
       </c>
       <c r="W71" s="0">
         <v>0</v>
@@ -2494,15 +2494,15 @@
     </row>
     <row outlineLevel="0" r="72">
       <c r="A72" s="0">
-        <v>103</v>
+        <v>131</v>
       </c>
       <c r="B72" s="0" t="inlineStr">
         <is>
-          <t>IDBR</t>
+          <t>IABAS</t>
         </is>
       </c>
       <c r="V72" s="1">
-        <v>43595</v>
+        <v>43937</v>
       </c>
       <c r="W72" s="0">
         <v>0</v>
@@ -2522,15 +2522,15 @@
     </row>
     <row outlineLevel="0" r="73">
       <c r="A73" s="0">
-        <v>165</v>
+        <v>103</v>
       </c>
       <c r="B73" s="0" t="inlineStr">
         <is>
-          <t>IFOOD</t>
+          <t>IDBR</t>
         </is>
       </c>
       <c r="V73" s="1">
-        <v>44575</v>
+        <v>43595</v>
       </c>
       <c r="W73" s="0">
         <v>0</v>
@@ -2550,15 +2550,15 @@
     </row>
     <row outlineLevel="0" r="74">
       <c r="A74" s="0">
-        <v>138</v>
+        <v>165</v>
       </c>
       <c r="B74" s="0" t="inlineStr">
         <is>
-          <t>INFOVIEW</t>
+          <t>IFOOD</t>
         </is>
       </c>
       <c r="V74" s="1">
-        <v>44223</v>
+        <v>44575</v>
       </c>
       <c r="W74" s="0">
         <v>0</v>
@@ -2578,15 +2578,15 @@
     </row>
     <row outlineLevel="0" r="75">
       <c r="A75" s="0">
-        <v>1</v>
+        <v>138</v>
       </c>
       <c r="B75" s="0" t="inlineStr">
         <is>
-          <t>ITAIPAVA</t>
+          <t>INFOVIEW</t>
         </is>
       </c>
       <c r="V75" s="1">
-        <v>42117</v>
+        <v>44223</v>
       </c>
       <c r="W75" s="0">
         <v>0</v>
@@ -2606,15 +2606,15 @@
     </row>
     <row outlineLevel="0" r="76">
       <c r="A76" s="0">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B76" s="0" t="inlineStr">
         <is>
-          <t>ITAU</t>
+          <t>ITAIPAVA</t>
         </is>
       </c>
       <c r="V76" s="1">
-        <v>42171</v>
+        <v>42117</v>
       </c>
       <c r="W76" s="0">
         <v>0</v>
@@ -2634,15 +2634,15 @@
     </row>
     <row outlineLevel="0" r="77">
       <c r="A77" s="0">
-        <v>102</v>
+        <v>10</v>
       </c>
       <c r="B77" s="0" t="inlineStr">
         <is>
-          <t>JONATHAS - WEB (PROCESSO)</t>
+          <t>ITAU</t>
         </is>
       </c>
       <c r="V77" s="1">
-        <v>43593</v>
+        <v>42171</v>
       </c>
       <c r="W77" s="0">
         <v>0</v>
@@ -2662,15 +2662,15 @@
     </row>
     <row outlineLevel="0" r="78">
       <c r="A78" s="0">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="B78" s="0" t="inlineStr">
         <is>
-          <t>LANDEIRA</t>
+          <t>JONATHAS - WEB (PROCESSO)</t>
         </is>
       </c>
       <c r="V78" s="1">
-        <v>43067</v>
+        <v>43593</v>
       </c>
       <c r="W78" s="0">
         <v>0</v>
@@ -2690,15 +2690,15 @@
     </row>
     <row outlineLevel="0" r="79">
       <c r="A79" s="0">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="B79" s="0" t="inlineStr">
         <is>
-          <t>LOWES</t>
+          <t>LANDEIRA</t>
         </is>
       </c>
       <c r="V79" s="1">
-        <v>42678</v>
+        <v>43067</v>
       </c>
       <c r="W79" s="0">
         <v>0</v>
@@ -2718,15 +2718,15 @@
     </row>
     <row outlineLevel="0" r="80">
       <c r="A80" s="0">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="B80" s="0" t="inlineStr">
         <is>
-          <t>LUCCE</t>
+          <t>LOWES</t>
         </is>
       </c>
       <c r="V80" s="1">
-        <v>42220</v>
+        <v>42678</v>
       </c>
       <c r="W80" s="0">
         <v>0</v>
@@ -2746,15 +2746,15 @@
     </row>
     <row outlineLevel="0" r="81">
       <c r="A81" s="0">
-        <v>134</v>
+        <v>18</v>
       </c>
       <c r="B81" s="0" t="inlineStr">
         <is>
-          <t>LUFE</t>
+          <t>LUCCE</t>
         </is>
       </c>
       <c r="V81" s="1">
-        <v>44154</v>
+        <v>42220</v>
       </c>
       <c r="W81" s="0">
         <v>0</v>
@@ -2774,15 +2774,15 @@
     </row>
     <row outlineLevel="0" r="82">
       <c r="A82" s="0">
-        <v>57</v>
+        <v>134</v>
       </c>
       <c r="B82" s="0" t="inlineStr">
         <is>
-          <t>LUIZ AMARAL</t>
+          <t>LUFE</t>
         </is>
       </c>
       <c r="V82" s="1">
-        <v>42724</v>
+        <v>44154</v>
       </c>
       <c r="W82" s="0">
         <v>0</v>
@@ -2802,15 +2802,15 @@
     </row>
     <row outlineLevel="0" r="83">
       <c r="A83" s="0">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="B83" s="0" t="inlineStr">
         <is>
-          <t>LVHM</t>
+          <t>LUIZ AMARAL</t>
         </is>
       </c>
       <c r="V83" s="1">
-        <v>42193</v>
+        <v>42724</v>
       </c>
       <c r="W83" s="0">
         <v>0</v>
@@ -2830,15 +2830,15 @@
     </row>
     <row outlineLevel="0" r="84">
       <c r="A84" s="0">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B84" s="0" t="inlineStr">
         <is>
-          <t>LVMH</t>
+          <t>LVHM</t>
         </is>
       </c>
       <c r="V84" s="1">
-        <v>42355</v>
+        <v>42193</v>
       </c>
       <c r="W84" s="0">
         <v>0</v>
@@ -2858,15 +2858,15 @@
     </row>
     <row outlineLevel="0" r="85">
       <c r="A85" s="0">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B85" s="0" t="inlineStr">
         <is>
-          <t>MALAKA</t>
+          <t>LVMH</t>
         </is>
       </c>
       <c r="V85" s="1">
-        <v>42117</v>
+        <v>42355</v>
       </c>
       <c r="W85" s="0">
         <v>0</v>
@@ -2886,15 +2886,15 @@
     </row>
     <row outlineLevel="0" r="86">
       <c r="A86" s="0">
-        <v>167</v>
+        <v>2</v>
       </c>
       <c r="B86" s="0" t="inlineStr">
         <is>
-          <t>MARINA GIN</t>
+          <t>MALAKA</t>
         </is>
       </c>
       <c r="V86" s="1">
-        <v>44616</v>
+        <v>42117</v>
       </c>
       <c r="W86" s="0">
         <v>0</v>
@@ -2914,15 +2914,15 @@
     </row>
     <row outlineLevel="0" r="87">
       <c r="A87" s="0">
-        <v>21</v>
+        <v>167</v>
       </c>
       <c r="B87" s="0" t="inlineStr">
         <is>
-          <t>METRÓPOLE</t>
+          <t>MARINA GIN</t>
         </is>
       </c>
       <c r="V87" s="1">
-        <v>42242</v>
+        <v>44616</v>
       </c>
       <c r="W87" s="0">
         <v>0</v>
@@ -2942,15 +2942,15 @@
     </row>
     <row outlineLevel="0" r="88">
       <c r="A88" s="0">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="B88" s="0" t="inlineStr">
         <is>
-          <t>MOET HENNESSY</t>
+          <t>METRÓPOLE</t>
         </is>
       </c>
       <c r="V88" s="1">
-        <v>42446</v>
+        <v>42242</v>
       </c>
       <c r="W88" s="0">
         <v>0</v>
@@ -2970,60 +2970,15 @@
     </row>
     <row outlineLevel="0" r="89">
       <c r="A89" s="0">
-        <v>99</v>
+        <v>35</v>
       </c>
       <c r="B89" s="0" t="inlineStr">
         <is>
-          <t>MOSTARDA PRODUÇÕES E EVENTOS LTDA - ME</t>
-        </is>
-      </c>
-      <c r="C89" s="0" t="inlineStr">
-        <is>
-          <t>MOSTARDA PRODUÇOES</t>
-        </is>
-      </c>
-      <c r="F89" s="0" t="inlineStr">
-        <is>
-          <t>RUA LEANDRO MARTINS, 10 SALA 902</t>
-        </is>
-      </c>
-      <c r="G89" s="0" t="inlineStr">
-        <is>
-          <t>CENTRO</t>
-        </is>
-      </c>
-      <c r="H89" s="0" t="inlineStr">
-        <is>
-          <t>RIO DE JANEIRO</t>
-        </is>
-      </c>
-      <c r="I89" s="0" t="inlineStr">
-        <is>
-          <t>RJ</t>
-        </is>
-      </c>
-      <c r="J89" s="0" t="inlineStr">
-        <is>
-          <t>20080-070</t>
-        </is>
-      </c>
-      <c r="L89" s="0" t="inlineStr">
-        <is>
-          <t>18.381.709/0001-40</t>
-        </is>
-      </c>
-      <c r="M89" s="0" t="inlineStr">
-        <is>
-          <t>ISENTO</t>
-        </is>
-      </c>
-      <c r="N89" s="0" t="inlineStr">
-        <is>
-          <t>0.582.179-7</t>
+          <t>MOET HENNESSY</t>
         </is>
       </c>
       <c r="V89" s="1">
-        <v>43560</v>
+        <v>42446</v>
       </c>
       <c r="W89" s="0">
         <v>0</v>
@@ -3043,20 +2998,60 @@
     </row>
     <row outlineLevel="0" r="90">
       <c r="A90" s="0">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="B90" s="0" t="inlineStr">
         <is>
-          <t>NATHÁLIA QUINTANS</t>
-        </is>
-      </c>
-      <c r="O90" s="0" t="inlineStr">
-        <is>
-          <t>11010906771</t>
+          <t>MOSTARDA PRODUÇÕES E EVENTOS LTDA - ME</t>
+        </is>
+      </c>
+      <c r="C90" s="0" t="inlineStr">
+        <is>
+          <t>MOSTARDA PRODUÇOES</t>
+        </is>
+      </c>
+      <c r="F90" s="0" t="inlineStr">
+        <is>
+          <t>RUA LEANDRO MARTINS, 10 SALA 902</t>
+        </is>
+      </c>
+      <c r="G90" s="0" t="inlineStr">
+        <is>
+          <t>CENTRO</t>
+        </is>
+      </c>
+      <c r="H90" s="0" t="inlineStr">
+        <is>
+          <t>RIO DE JANEIRO</t>
+        </is>
+      </c>
+      <c r="I90" s="0" t="inlineStr">
+        <is>
+          <t>RJ</t>
+        </is>
+      </c>
+      <c r="J90" s="0" t="inlineStr">
+        <is>
+          <t>20080-070</t>
+        </is>
+      </c>
+      <c r="L90" s="0" t="inlineStr">
+        <is>
+          <t>18.381.709/0001-40</t>
+        </is>
+      </c>
+      <c r="M90" s="0" t="inlineStr">
+        <is>
+          <t>ISENTO</t>
+        </is>
+      </c>
+      <c r="N90" s="0" t="inlineStr">
+        <is>
+          <t>0.582.179-7</t>
         </is>
       </c>
       <c r="V90" s="1">
-        <v>43805</v>
+        <v>43560</v>
       </c>
       <c r="W90" s="0">
         <v>0</v>
@@ -3072,34 +3067,24 @@
       </c>
       <c r="AB90" s="0" t="b">
         <v>0</v>
-      </c>
-      <c r="AC90" s="0" t="inlineStr">
-        <is>
-          <t>SANTANDER</t>
-        </is>
-      </c>
-      <c r="AD90" s="0" t="inlineStr">
-        <is>
-          <t>3201</t>
-        </is>
-      </c>
-      <c r="AE90" s="0" t="inlineStr">
-        <is>
-          <t>1005067-3</t>
-        </is>
       </c>
     </row>
     <row outlineLevel="0" r="91">
       <c r="A91" s="0">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="B91" s="0" t="inlineStr">
         <is>
-          <t>NBA</t>
+          <t>NATHÁLIA QUINTANS</t>
+        </is>
+      </c>
+      <c r="O91" s="0" t="inlineStr">
+        <is>
+          <t>11010906771</t>
         </is>
       </c>
       <c r="V91" s="1">
-        <v>43566</v>
+        <v>43805</v>
       </c>
       <c r="W91" s="0">
         <v>0</v>
@@ -3115,19 +3100,34 @@
       </c>
       <c r="AB91" s="0" t="b">
         <v>0</v>
+      </c>
+      <c r="AC91" s="0" t="inlineStr">
+        <is>
+          <t>SANTANDER</t>
+        </is>
+      </c>
+      <c r="AD91" s="0" t="inlineStr">
+        <is>
+          <t>3201</t>
+        </is>
+      </c>
+      <c r="AE91" s="0" t="inlineStr">
+        <is>
+          <t>1005067-3</t>
+        </is>
       </c>
     </row>
     <row outlineLevel="0" r="92">
       <c r="A92" s="0">
-        <v>153</v>
+        <v>100</v>
       </c>
       <c r="B92" s="0" t="inlineStr">
         <is>
-          <t>ND AMERICANAS</t>
+          <t>NBA</t>
         </is>
       </c>
       <c r="V92" s="1">
-        <v>44419</v>
+        <v>43566</v>
       </c>
       <c r="W92" s="0">
         <v>0</v>
@@ -3147,15 +3147,15 @@
     </row>
     <row outlineLevel="0" r="93">
       <c r="A93" s="0">
-        <v>118</v>
+        <v>153</v>
       </c>
       <c r="B93" s="0" t="inlineStr">
         <is>
-          <t>NELIO/REGINA</t>
+          <t>ND AMERICANAS</t>
         </is>
       </c>
       <c r="V93" s="1">
-        <v>43802</v>
+        <v>44419</v>
       </c>
       <c r="W93" s="0">
         <v>0</v>
@@ -3170,20 +3170,20 @@
         <v>0</v>
       </c>
       <c r="AB93" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row outlineLevel="0" r="94">
       <c r="A94" s="0">
-        <v>160</v>
+        <v>118</v>
       </c>
       <c r="B94" s="0" t="inlineStr">
         <is>
-          <t>NETZA</t>
+          <t>NELIO/REGINA</t>
         </is>
       </c>
       <c r="V94" s="1">
-        <v>44483</v>
+        <v>43802</v>
       </c>
       <c r="W94" s="0">
         <v>0</v>
@@ -3198,20 +3198,20 @@
         <v>0</v>
       </c>
       <c r="AB94" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row outlineLevel="0" r="95">
       <c r="A95" s="0">
-        <v>8</v>
+        <v>160</v>
       </c>
       <c r="B95" s="0" t="inlineStr">
         <is>
-          <t>NIGHTRIO</t>
+          <t>NETZA</t>
         </is>
       </c>
       <c r="V95" s="1">
-        <v>42149</v>
+        <v>44483</v>
       </c>
       <c r="W95" s="0">
         <v>0</v>
@@ -3231,15 +3231,15 @@
     </row>
     <row outlineLevel="0" r="96">
       <c r="A96" s="0">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="B96" s="0" t="inlineStr">
         <is>
-          <t>NORMAL PRA GENTE</t>
+          <t>NIGHTRIO</t>
         </is>
       </c>
       <c r="V96" s="1">
-        <v>43524</v>
+        <v>42149</v>
       </c>
       <c r="W96" s="0">
         <v>0</v>
@@ -3259,15 +3259,15 @@
     </row>
     <row outlineLevel="0" r="97">
       <c r="A97" s="0">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="B97" s="0" t="inlineStr">
         <is>
-          <t>OLX</t>
+          <t>NORMAL PRA GENTE</t>
         </is>
       </c>
       <c r="V97" s="1">
-        <v>43326</v>
+        <v>43524</v>
       </c>
       <c r="W97" s="0">
         <v>0</v>
@@ -3287,15 +3287,15 @@
     </row>
     <row outlineLevel="0" r="98">
       <c r="A98" s="0">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="B98" s="0" t="inlineStr">
         <is>
-          <t>ORION BRANDING</t>
+          <t>OLX</t>
         </is>
       </c>
       <c r="V98" s="1">
-        <v>42635</v>
+        <v>43326</v>
       </c>
       <c r="W98" s="0">
         <v>0</v>
@@ -3315,15 +3315,15 @@
     </row>
     <row outlineLevel="0" r="99">
       <c r="A99" s="0">
-        <v>136</v>
+        <v>48</v>
       </c>
       <c r="B99" s="0" t="inlineStr">
         <is>
-          <t>ORLA RIO</t>
+          <t>ORION BRANDING</t>
         </is>
       </c>
       <c r="V99" s="1">
-        <v>44161</v>
+        <v>42635</v>
       </c>
       <c r="W99" s="0">
         <v>0</v>
@@ -3343,25 +3343,15 @@
     </row>
     <row outlineLevel="0" r="100">
       <c r="A100" s="0">
-        <v>108</v>
+        <v>136</v>
       </c>
       <c r="B100" s="0" t="inlineStr">
         <is>
-          <t>OS BATUTINHAS</t>
-        </is>
-      </c>
-      <c r="C100" s="0" t="inlineStr">
-        <is>
-          <t>OS BATUTINHAS ESPAÇO DE EDUC. INFANTIL LTDA</t>
-        </is>
-      </c>
-      <c r="L100" s="0" t="inlineStr">
-        <is>
-          <t>01.211.472/0001-56</t>
+          <t>ORLA RIO</t>
         </is>
       </c>
       <c r="V100" s="1">
-        <v>43651</v>
+        <v>44161</v>
       </c>
       <c r="W100" s="0">
         <v>0</v>
@@ -3381,15 +3371,25 @@
     </row>
     <row outlineLevel="0" r="101">
       <c r="A101" s="0">
-        <v>162</v>
+        <v>108</v>
       </c>
       <c r="B101" s="0" t="inlineStr">
         <is>
-          <t>OTALAB (CEREBRO)</t>
+          <t>OS BATUTINHAS</t>
+        </is>
+      </c>
+      <c r="C101" s="0" t="inlineStr">
+        <is>
+          <t>OS BATUTINHAS ESPAÇO DE EDUC. INFANTIL LTDA</t>
+        </is>
+      </c>
+      <c r="L101" s="0" t="inlineStr">
+        <is>
+          <t>01.211.472/0001-56</t>
         </is>
       </c>
       <c r="V101" s="1">
-        <v>44505</v>
+        <v>43651</v>
       </c>
       <c r="W101" s="0">
         <v>0</v>
@@ -3409,20 +3409,15 @@
     </row>
     <row outlineLevel="0" r="102">
       <c r="A102" s="0">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="B102" s="0" t="inlineStr">
         <is>
-          <t>ÓTIMA CONCESSIONÁRIA</t>
-        </is>
-      </c>
-      <c r="U102" s="0" t="inlineStr">
-        <is>
-          <t>anapaula.couto@otima.com</t>
+          <t>OTALAB (CEREBRO)</t>
         </is>
       </c>
       <c r="V102" s="1">
-        <v>44379</v>
+        <v>44505</v>
       </c>
       <c r="W102" s="0">
         <v>0</v>
@@ -3442,55 +3437,20 @@
     </row>
     <row outlineLevel="0" r="103">
       <c r="A103" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B103" s="0" t="inlineStr">
         <is>
-          <t>ÓTIMA CONCESSIONÁRIA DE EXPLORAÇÃO MOBILIÁRIO URBANO LTDA</t>
-        </is>
-      </c>
-      <c r="F103" s="0" t="inlineStr">
-        <is>
-          <t>RUA MOFARREJ, 1298</t>
-        </is>
-      </c>
-      <c r="G103" s="0" t="inlineStr">
-        <is>
-          <t>VILA LEOPOLDINA</t>
-        </is>
-      </c>
-      <c r="H103" s="0" t="inlineStr">
-        <is>
-          <t>SÃO PAULO</t>
-        </is>
-      </c>
-      <c r="I103" s="0" t="inlineStr">
-        <is>
-          <t>SP</t>
-        </is>
-      </c>
-      <c r="J103" s="0" t="inlineStr">
-        <is>
-          <t>06311-000</t>
-        </is>
-      </c>
-      <c r="L103" s="0" t="inlineStr">
-        <is>
-          <t>17.104.815/0001-13</t>
-        </is>
-      </c>
-      <c r="N103" s="0" t="inlineStr">
-        <is>
-          <t>4645058-0</t>
+          <t>ÓTIMA CONCESSIONÁRIA</t>
         </is>
       </c>
       <c r="U103" s="0" t="inlineStr">
         <is>
-          <t>anapaula.couto@otima.com (FINANCEIRO)</t>
+          <t>anapaula.couto@otima.com</t>
         </is>
       </c>
       <c r="V103" s="1">
-        <v>44347</v>
+        <v>44379</v>
       </c>
       <c r="W103" s="0">
         <v>0</v>
@@ -3510,15 +3470,55 @@
     </row>
     <row outlineLevel="0" r="104">
       <c r="A104" s="0">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B104" s="0" t="inlineStr">
         <is>
-          <t>PAD BH</t>
+          <t>ÓTIMA CONCESSIONÁRIA DE EXPLORAÇÃO MOBILIÁRIO URBANO LTDA</t>
+        </is>
+      </c>
+      <c r="F104" s="0" t="inlineStr">
+        <is>
+          <t>RUA MOFARREJ, 1298</t>
+        </is>
+      </c>
+      <c r="G104" s="0" t="inlineStr">
+        <is>
+          <t>VILA LEOPOLDINA</t>
+        </is>
+      </c>
+      <c r="H104" s="0" t="inlineStr">
+        <is>
+          <t>SÃO PAULO</t>
+        </is>
+      </c>
+      <c r="I104" s="0" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="J104" s="0" t="inlineStr">
+        <is>
+          <t>06311-000</t>
+        </is>
+      </c>
+      <c r="L104" s="0" t="inlineStr">
+        <is>
+          <t>17.104.815/0001-13</t>
+        </is>
+      </c>
+      <c r="N104" s="0" t="inlineStr">
+        <is>
+          <t>4645058-0</t>
+        </is>
+      </c>
+      <c r="U104" s="0" t="inlineStr">
+        <is>
+          <t>anapaula.couto@otima.com (FINANCEIRO)</t>
         </is>
       </c>
       <c r="V104" s="1">
-        <v>44294</v>
+        <v>44347</v>
       </c>
       <c r="W104" s="0">
         <v>0</v>
@@ -3538,15 +3538,15 @@
     </row>
     <row outlineLevel="0" r="105">
       <c r="A105" s="0">
-        <v>39</v>
+        <v>143</v>
       </c>
       <c r="B105" s="0" t="inlineStr">
         <is>
-          <t>PAULO DE CASTRO</t>
+          <t>PAD BH</t>
         </is>
       </c>
       <c r="V105" s="1">
-        <v>42471</v>
+        <v>44294</v>
       </c>
       <c r="W105" s="0">
         <v>0</v>
@@ -3566,15 +3566,15 @@
     </row>
     <row outlineLevel="0" r="106">
       <c r="A106" s="0">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="B106" s="0" t="inlineStr">
         <is>
-          <t>PEDRO GUIMARÃES</t>
+          <t>PAULO DE CASTRO</t>
         </is>
       </c>
       <c r="V106" s="1">
-        <v>42136</v>
+        <v>42471</v>
       </c>
       <c r="W106" s="0">
         <v>0</v>
@@ -3594,15 +3594,15 @@
     </row>
     <row outlineLevel="0" r="107">
       <c r="A107" s="0">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="B107" s="0" t="inlineStr">
         <is>
-          <t>PEDRO VILELA</t>
+          <t>PEDRO GUIMARÃES</t>
         </is>
       </c>
       <c r="V107" s="1">
-        <v>42359</v>
+        <v>42136</v>
       </c>
       <c r="W107" s="0">
         <v>0</v>
@@ -3622,15 +3622,15 @@
     </row>
     <row outlineLevel="0" r="108">
       <c r="A108" s="0">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B108" s="0" t="inlineStr">
         <is>
-          <t>Pernod Ricard</t>
+          <t>PEDRO VILELA</t>
         </is>
       </c>
       <c r="V108" s="1">
-        <v>42135</v>
+        <v>42359</v>
       </c>
       <c r="W108" s="0">
         <v>0</v>
@@ -3650,15 +3650,15 @@
     </row>
     <row outlineLevel="0" r="109">
       <c r="A109" s="0">
-        <v>126</v>
+        <v>5</v>
       </c>
       <c r="B109" s="0" t="inlineStr">
         <is>
-          <t>PLAY 9</t>
+          <t>Pernod Ricard</t>
         </is>
       </c>
       <c r="V109" s="1">
-        <v>43846</v>
+        <v>42135</v>
       </c>
       <c r="W109" s="0">
         <v>0</v>
@@ -3678,15 +3678,15 @@
     </row>
     <row outlineLevel="0" r="110">
       <c r="A110" s="0">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B110" s="0" t="inlineStr">
         <is>
-          <t>PRODUTORA IDEIA REAL</t>
+          <t>PLAY 9</t>
         </is>
       </c>
       <c r="V110" s="1">
-        <v>43900</v>
+        <v>43846</v>
       </c>
       <c r="W110" s="0">
         <v>0</v>
@@ -3706,15 +3706,15 @@
     </row>
     <row outlineLevel="0" r="111">
       <c r="A111" s="0">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="B111" s="0" t="inlineStr">
         <is>
-          <t>REBECA KAIZER</t>
+          <t>PRODUTORA IDEIA REAL</t>
         </is>
       </c>
       <c r="V111" s="1">
-        <v>43821</v>
+        <v>43900</v>
       </c>
       <c r="W111" s="0">
         <v>0</v>
@@ -3734,15 +3734,15 @@
     </row>
     <row outlineLevel="0" r="112">
       <c r="A112" s="0">
-        <v>43</v>
+        <v>124</v>
       </c>
       <c r="B112" s="0" t="inlineStr">
         <is>
-          <t>RED BULL</t>
+          <t>REBECA KAIZER</t>
         </is>
       </c>
       <c r="V112" s="1">
-        <v>42511</v>
+        <v>43821</v>
       </c>
       <c r="W112" s="0">
         <v>0</v>
@@ -3762,15 +3762,15 @@
     </row>
     <row outlineLevel="0" r="113">
       <c r="A113" s="0">
-        <v>137</v>
+        <v>43</v>
       </c>
       <c r="B113" s="0" t="inlineStr">
         <is>
-          <t>RED DOOR</t>
+          <t>RED BULL</t>
         </is>
       </c>
       <c r="V113" s="1">
-        <v>44180</v>
+        <v>42511</v>
       </c>
       <c r="W113" s="0">
         <v>0</v>
@@ -3790,15 +3790,15 @@
     </row>
     <row outlineLevel="0" r="114">
       <c r="A114" s="0">
-        <v>84</v>
+        <v>137</v>
       </c>
       <c r="B114" s="0" t="inlineStr">
         <is>
-          <t>RESERVA</t>
+          <t>RED DOOR</t>
         </is>
       </c>
       <c r="V114" s="1">
-        <v>43154</v>
+        <v>44180</v>
       </c>
       <c r="W114" s="0">
         <v>0</v>
@@ -3818,15 +3818,15 @@
     </row>
     <row outlineLevel="0" r="115">
       <c r="A115" s="0">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="B115" s="0" t="inlineStr">
         <is>
-          <t>RIACHUELO IPANEMA</t>
+          <t>RESERVA</t>
         </is>
       </c>
       <c r="V115" s="1">
-        <v>42865</v>
+        <v>43154</v>
       </c>
       <c r="W115" s="0">
         <v>0</v>
@@ -3846,15 +3846,15 @@
     </row>
     <row outlineLevel="0" r="116">
       <c r="A116" s="0">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="B116" s="0" t="inlineStr">
         <is>
-          <t>RIGGAR</t>
+          <t>RIACHUELO IPANEMA</t>
         </is>
       </c>
       <c r="V116" s="1">
-        <v>43048</v>
+        <v>42865</v>
       </c>
       <c r="W116" s="0">
         <v>0</v>
@@ -3874,15 +3874,15 @@
     </row>
     <row outlineLevel="0" r="117">
       <c r="A117" s="0">
-        <v>117</v>
+        <v>79</v>
       </c>
       <c r="B117" s="0" t="inlineStr">
         <is>
-          <t>RIOZOO</t>
+          <t>RIGGAR</t>
         </is>
       </c>
       <c r="V117" s="1">
-        <v>43776</v>
+        <v>43048</v>
       </c>
       <c r="W117" s="0">
         <v>0</v>
@@ -3902,15 +3902,15 @@
     </row>
     <row outlineLevel="0" r="118">
       <c r="A118" s="0">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="B118" s="0" t="inlineStr">
         <is>
-          <t>ROCK IN RIO</t>
+          <t>RIOZOO</t>
         </is>
       </c>
       <c r="V118" s="1">
-        <v>42982</v>
+        <v>43776</v>
       </c>
       <c r="W118" s="0">
         <v>0</v>
@@ -3930,15 +3930,15 @@
     </row>
     <row outlineLevel="0" r="119">
       <c r="A119" s="0">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="B119" s="0" t="inlineStr">
         <is>
-          <t>RODRIGO LAMPREIA</t>
+          <t>ROCK IN RIO</t>
         </is>
       </c>
       <c r="V119" s="1">
-        <v>42435</v>
+        <v>42982</v>
       </c>
       <c r="W119" s="0">
         <v>0</v>
@@ -3958,15 +3958,15 @@
     </row>
     <row outlineLevel="0" r="120">
       <c r="A120" s="0">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B120" s="0" t="inlineStr">
         <is>
-          <t>SCHEEEINS</t>
+          <t>RODRIGO LAMPREIA</t>
         </is>
       </c>
       <c r="V120" s="1">
-        <v>42243</v>
+        <v>42435</v>
       </c>
       <c r="W120" s="0">
         <v>0</v>
@@ -3986,15 +3986,15 @@
     </row>
     <row outlineLevel="0" r="121">
       <c r="A121" s="0">
-        <v>127</v>
+        <v>22</v>
       </c>
       <c r="B121" s="0" t="inlineStr">
         <is>
-          <t>SCORE GROUP (SP)</t>
+          <t>SCHEEEINS</t>
         </is>
       </c>
       <c r="V121" s="1">
-        <v>43852</v>
+        <v>42243</v>
       </c>
       <c r="W121" s="0">
         <v>0</v>
@@ -4014,15 +4014,15 @@
     </row>
     <row outlineLevel="0" r="122">
       <c r="A122" s="0">
-        <v>168</v>
+        <v>127</v>
       </c>
       <c r="B122" s="0" t="inlineStr">
         <is>
-          <t>SEBASTIAN</t>
+          <t>SCORE GROUP (SP)</t>
         </is>
       </c>
       <c r="V122" s="1">
-        <v>44634</v>
+        <v>43852</v>
       </c>
       <c r="W122" s="0">
         <v>0</v>
@@ -4042,15 +4042,15 @@
     </row>
     <row outlineLevel="0" r="123">
       <c r="A123" s="0">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="B123" s="0" t="inlineStr">
         <is>
-          <t>SEM EFEITO</t>
+          <t>SEBASTIAN</t>
         </is>
       </c>
       <c r="V123" s="1">
-        <v>44379</v>
+        <v>44634</v>
       </c>
       <c r="W123" s="0">
         <v>0</v>
@@ -4070,15 +4070,15 @@
     </row>
     <row outlineLevel="0" r="124">
       <c r="A124" s="0">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="B124" s="0" t="inlineStr">
         <is>
-          <t>SEU VIDAL</t>
+          <t>SEM EFEITO</t>
         </is>
       </c>
       <c r="V124" s="1">
-        <v>42881</v>
+        <v>44379</v>
       </c>
       <c r="W124" s="0">
         <v>0</v>
@@ -4098,15 +4098,15 @@
     </row>
     <row outlineLevel="0" r="125">
       <c r="A125" s="0">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="B125" s="0" t="inlineStr">
         <is>
-          <t>SHERPA42</t>
+          <t>SEU VIDAL</t>
         </is>
       </c>
       <c r="V125" s="1">
-        <v>42677</v>
+        <v>42881</v>
       </c>
       <c r="W125" s="0">
         <v>0</v>
@@ -4126,15 +4126,15 @@
     </row>
     <row outlineLevel="0" r="126">
       <c r="A126" s="0">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B126" s="0" t="inlineStr">
         <is>
-          <t>SHOPPING BOULEVARD</t>
+          <t>SHERPA42</t>
         </is>
       </c>
       <c r="V126" s="1">
-        <v>42821</v>
+        <v>42677</v>
       </c>
       <c r="W126" s="0">
         <v>0</v>
@@ -4154,15 +4154,15 @@
     </row>
     <row outlineLevel="0" r="127">
       <c r="A127" s="0">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B127" s="0" t="inlineStr">
         <is>
-          <t>SHOPPING NOVA AMÉRICA</t>
+          <t>SHOPPING BOULEVARD</t>
         </is>
       </c>
       <c r="V127" s="1">
-        <v>42863</v>
+        <v>42821</v>
       </c>
       <c r="W127" s="0">
         <v>0</v>
@@ -4182,20 +4182,15 @@
     </row>
     <row outlineLevel="0" r="128">
       <c r="A128" s="0">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="B128" s="0" t="inlineStr">
         <is>
-          <t>SONHO DOS PÉS</t>
-        </is>
-      </c>
-      <c r="D128" s="0" t="inlineStr">
-        <is>
-          <t>Bárbara Soledade</t>
+          <t>SHOPPING NOVA AMÉRICA</t>
         </is>
       </c>
       <c r="V128" s="1">
-        <v>43752</v>
+        <v>42863</v>
       </c>
       <c r="W128" s="0">
         <v>0</v>
@@ -4215,50 +4210,20 @@
     </row>
     <row outlineLevel="0" r="129">
       <c r="A129" s="0">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="B129" s="0" t="inlineStr">
         <is>
-          <t>SORRIA</t>
-        </is>
-      </c>
-      <c r="C129" s="0" t="inlineStr">
-        <is>
-          <t>SORRIA</t>
-        </is>
-      </c>
-      <c r="F129" s="0" t="inlineStr">
-        <is>
-          <t>AV DAS HORTÊNCIAS,</t>
-        </is>
-      </c>
-      <c r="G129" s="0" t="inlineStr">
-        <is>
-          <t>AVENIDA CENTRAL</t>
-        </is>
-      </c>
-      <c r="H129" s="0" t="inlineStr">
-        <is>
-          <t>GRAMADO</t>
-        </is>
-      </c>
-      <c r="I129" s="0" t="inlineStr">
-        <is>
-          <t>RS</t>
-        </is>
-      </c>
-      <c r="J129" s="0" t="inlineStr">
-        <is>
-          <t>95670-000</t>
-        </is>
-      </c>
-      <c r="L129" s="0" t="inlineStr">
-        <is>
-          <t>34.573.787/0001-00</t>
+          <t>SONHO DOS PÉS</t>
+        </is>
+      </c>
+      <c r="D129" s="0" t="inlineStr">
+        <is>
+          <t>Bárbara Soledade</t>
         </is>
       </c>
       <c r="V129" s="1">
-        <v>44057</v>
+        <v>43752</v>
       </c>
       <c r="W129" s="0">
         <v>0</v>
@@ -4278,65 +4243,50 @@
     </row>
     <row outlineLevel="0" r="130">
       <c r="A130" s="0">
-        <v>164</v>
+        <v>133</v>
       </c>
       <c r="B130" s="0" t="inlineStr">
         <is>
-          <t>SPANTA NENEM</t>
+          <t>SORRIA</t>
         </is>
       </c>
       <c r="C130" s="0" t="inlineStr">
         <is>
-          <t>ASSOC E GR. RECR. BL CANAVALESCO SPANTA NENEM</t>
+          <t>SORRIA</t>
         </is>
       </c>
       <c r="F130" s="0" t="inlineStr">
         <is>
-          <t>RUA BARÃO DE LUCENA,32</t>
+          <t>AV DAS HORTÊNCIAS,</t>
         </is>
       </c>
       <c r="G130" s="0" t="inlineStr">
         <is>
-          <t>BOTAFOGO</t>
+          <t>AVENIDA CENTRAL</t>
         </is>
       </c>
       <c r="H130" s="0" t="inlineStr">
         <is>
-          <t>RIO DE JANEIRO</t>
+          <t>GRAMADO</t>
         </is>
       </c>
       <c r="I130" s="0" t="inlineStr">
         <is>
-          <t>RJ</t>
+          <t>RS</t>
         </is>
       </c>
       <c r="J130" s="0" t="inlineStr">
         <is>
-          <t>22260-020</t>
+          <t>95670-000</t>
         </is>
       </c>
       <c r="L130" s="0" t="inlineStr">
         <is>
-          <t>07.094.273/0001-91</t>
-        </is>
-      </c>
-      <c r="M130" s="0" t="inlineStr">
-        <is>
-          <t>ISENTA</t>
-        </is>
-      </c>
-      <c r="N130" s="0" t="inlineStr">
-        <is>
-          <t>0497916-8</t>
-        </is>
-      </c>
-      <c r="Q130" s="0" t="inlineStr">
-        <is>
-          <t>21997276709</t>
+          <t>34.573.787/0001-00</t>
         </is>
       </c>
       <c r="V130" s="1">
-        <v>44547</v>
+        <v>44057</v>
       </c>
       <c r="W130" s="0">
         <v>0</v>
@@ -4356,15 +4306,65 @@
     </row>
     <row outlineLevel="0" r="131">
       <c r="A131" s="0">
-        <v>115</v>
+        <v>164</v>
       </c>
       <c r="B131" s="0" t="inlineStr">
         <is>
-          <t>SPOLETO</t>
+          <t>SPANTA NENEM</t>
+        </is>
+      </c>
+      <c r="C131" s="0" t="inlineStr">
+        <is>
+          <t>ASSOC E GR. RECR. BL CANAVALESCO SPANTA NENEM</t>
+        </is>
+      </c>
+      <c r="F131" s="0" t="inlineStr">
+        <is>
+          <t>RUA BARÃO DE LUCENA,32</t>
+        </is>
+      </c>
+      <c r="G131" s="0" t="inlineStr">
+        <is>
+          <t>BOTAFOGO</t>
+        </is>
+      </c>
+      <c r="H131" s="0" t="inlineStr">
+        <is>
+          <t>RIO DE JANEIRO</t>
+        </is>
+      </c>
+      <c r="I131" s="0" t="inlineStr">
+        <is>
+          <t>RJ</t>
+        </is>
+      </c>
+      <c r="J131" s="0" t="inlineStr">
+        <is>
+          <t>22260-020</t>
+        </is>
+      </c>
+      <c r="L131" s="0" t="inlineStr">
+        <is>
+          <t>07.094.273/0001-91</t>
+        </is>
+      </c>
+      <c r="M131" s="0" t="inlineStr">
+        <is>
+          <t>ISENTA</t>
+        </is>
+      </c>
+      <c r="N131" s="0" t="inlineStr">
+        <is>
+          <t>0497916-8</t>
+        </is>
+      </c>
+      <c r="Q131" s="0" t="inlineStr">
+        <is>
+          <t>21997276709</t>
         </is>
       </c>
       <c r="V131" s="1">
-        <v>43766</v>
+        <v>44547</v>
       </c>
       <c r="W131" s="0">
         <v>0</v>
@@ -4384,15 +4384,15 @@
     </row>
     <row outlineLevel="0" r="132">
       <c r="A132" s="0">
-        <v>71</v>
+        <v>115</v>
       </c>
       <c r="B132" s="0" t="inlineStr">
         <is>
-          <t>SRCOM</t>
+          <t>SPOLETO</t>
         </is>
       </c>
       <c r="V132" s="1">
-        <v>42926</v>
+        <v>43766</v>
       </c>
       <c r="W132" s="0">
         <v>0</v>
@@ -4412,15 +4412,15 @@
     </row>
     <row outlineLevel="0" r="133">
       <c r="A133" s="0">
-        <v>159</v>
+        <v>71</v>
       </c>
       <c r="B133" s="0" t="inlineStr">
         <is>
-          <t>STAND EVE EMBAER</t>
+          <t>SRCOM</t>
         </is>
       </c>
       <c r="V133" s="1">
-        <v>44483</v>
+        <v>42926</v>
       </c>
       <c r="W133" s="0">
         <v>0</v>
@@ -4440,15 +4440,15 @@
     </row>
     <row outlineLevel="0" r="134">
       <c r="A134" s="0">
-        <v>7</v>
+        <v>159</v>
       </c>
       <c r="B134" s="0" t="inlineStr">
         <is>
-          <t>TAG</t>
+          <t>STAND EVE EMBAER</t>
         </is>
       </c>
       <c r="V134" s="1">
-        <v>42149</v>
+        <v>44483</v>
       </c>
       <c r="W134" s="0">
         <v>0</v>
@@ -4468,15 +4468,15 @@
     </row>
     <row outlineLevel="0" r="135">
       <c r="A135" s="0">
-        <v>92</v>
+        <v>7</v>
       </c>
       <c r="B135" s="0" t="inlineStr">
         <is>
-          <t>TAKE 4 CONTENT</t>
+          <t>TAG</t>
         </is>
       </c>
       <c r="V135" s="1">
-        <v>43375</v>
+        <v>42149</v>
       </c>
       <c r="W135" s="0">
         <v>0</v>
@@ -4496,15 +4496,15 @@
     </row>
     <row outlineLevel="0" r="136">
       <c r="A136" s="0">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="B136" s="0" t="inlineStr">
         <is>
-          <t>TESTE</t>
+          <t>TAKE 4 CONTENT</t>
         </is>
       </c>
       <c r="V136" s="1">
-        <v>42178</v>
+        <v>43375</v>
       </c>
       <c r="W136" s="0">
         <v>0</v>
@@ -4524,15 +4524,15 @@
     </row>
     <row outlineLevel="0" r="137">
       <c r="A137" s="0">
-        <v>111</v>
+        <v>14</v>
       </c>
       <c r="B137" s="0" t="inlineStr">
         <is>
-          <t>THIAGO P PACHECO</t>
+          <t>TESTE</t>
         </is>
       </c>
       <c r="V137" s="1">
-        <v>43706</v>
+        <v>42178</v>
       </c>
       <c r="W137" s="0">
         <v>0</v>
@@ -4552,15 +4552,15 @@
     </row>
     <row outlineLevel="0" r="138">
       <c r="A138" s="0">
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="B138" s="0" t="inlineStr">
         <is>
-          <t>TWELVE MKT</t>
+          <t>THIAGO P PACHECO</t>
         </is>
       </c>
       <c r="V138" s="1">
-        <v>44321</v>
+        <v>43706</v>
       </c>
       <c r="W138" s="0">
         <v>0</v>
@@ -4580,15 +4580,15 @@
     </row>
     <row outlineLevel="0" r="139">
       <c r="A139" s="0">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B139" s="0" t="inlineStr">
         <is>
-          <t>TWELVE SPORTS &amp; MARKETING LT</t>
+          <t>TWELVE MKT</t>
         </is>
       </c>
       <c r="V139" s="1">
-        <v>44231</v>
+        <v>44321</v>
       </c>
       <c r="W139" s="0">
         <v>0</v>
@@ -4608,15 +4608,15 @@
     </row>
     <row outlineLevel="0" r="140">
       <c r="A140" s="0">
-        <v>98</v>
+        <v>139</v>
       </c>
       <c r="B140" s="0" t="inlineStr">
         <is>
-          <t>UEFA</t>
+          <t>TWELVE SPORTS &amp; MARKETING LT</t>
         </is>
       </c>
       <c r="V140" s="1">
-        <v>43539</v>
+        <v>44231</v>
       </c>
       <c r="W140" s="0">
         <v>0</v>
@@ -4636,15 +4636,15 @@
     </row>
     <row outlineLevel="0" r="141">
       <c r="A141" s="0">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="B141" s="0" t="inlineStr">
         <is>
-          <t>UMA UMA</t>
+          <t>UEFA</t>
         </is>
       </c>
       <c r="V141" s="1">
-        <v>43011</v>
+        <v>43539</v>
       </c>
       <c r="W141" s="0">
         <v>0</v>
@@ -4664,15 +4664,15 @@
     </row>
     <row outlineLevel="0" r="142">
       <c r="A142" s="0">
-        <v>140</v>
+        <v>77</v>
       </c>
       <c r="B142" s="0" t="inlineStr">
         <is>
-          <t>UNLIMITED IDEIAS</t>
+          <t>UMA UMA</t>
         </is>
       </c>
       <c r="V142" s="1">
-        <v>44250</v>
+        <v>43011</v>
       </c>
       <c r="W142" s="0">
         <v>0</v>
@@ -4692,15 +4692,15 @@
     </row>
     <row outlineLevel="0" r="143">
       <c r="A143" s="0">
-        <v>12</v>
+        <v>140</v>
       </c>
       <c r="B143" s="0" t="inlineStr">
         <is>
-          <t>UTILIZAR</t>
+          <t>UNLIMITED IDEIAS</t>
         </is>
       </c>
       <c r="V143" s="1">
-        <v>42173</v>
+        <v>44250</v>
       </c>
       <c r="W143" s="0">
         <v>0</v>
@@ -4720,15 +4720,15 @@
     </row>
     <row outlineLevel="0" r="144">
       <c r="A144" s="0">
-        <v>169</v>
+        <v>12</v>
       </c>
       <c r="B144" s="0" t="inlineStr">
         <is>
-          <t>V3A</t>
+          <t>UTILIZAR</t>
         </is>
       </c>
       <c r="V144" s="1">
-        <v>44645</v>
+        <v>42173</v>
       </c>
       <c r="W144" s="0">
         <v>0</v>
@@ -4748,15 +4748,15 @@
     </row>
     <row outlineLevel="0" r="145">
       <c r="A145" s="0">
-        <v>24</v>
+        <v>169</v>
       </c>
       <c r="B145" s="0" t="inlineStr">
         <is>
-          <t>VAL LASTRES</t>
+          <t>V3A</t>
         </is>
       </c>
       <c r="V145" s="1">
-        <v>42271</v>
+        <v>44645</v>
       </c>
       <c r="W145" s="0">
         <v>0</v>
@@ -4776,15 +4776,15 @@
     </row>
     <row outlineLevel="0" r="146">
       <c r="A146" s="0">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B146" s="0" t="inlineStr">
         <is>
-          <t>VAMBORA</t>
+          <t>VAL LASTRES</t>
         </is>
       </c>
       <c r="V146" s="1">
-        <v>42191</v>
+        <v>42271</v>
       </c>
       <c r="W146" s="0">
         <v>0</v>
@@ -4804,15 +4804,15 @@
     </row>
     <row outlineLevel="0" r="147">
       <c r="A147" s="0">
-        <v>112</v>
+        <v>15</v>
       </c>
       <c r="B147" s="0" t="inlineStr">
         <is>
-          <t>VIBES &amp; TALZ</t>
+          <t>VAMBORA</t>
         </is>
       </c>
       <c r="V147" s="1">
-        <v>43713</v>
+        <v>42191</v>
       </c>
       <c r="W147" s="0">
         <v>0</v>
@@ -4832,15 +4832,15 @@
     </row>
     <row outlineLevel="0" r="148">
       <c r="A148" s="0">
-        <v>73</v>
+        <v>112</v>
       </c>
       <c r="B148" s="0" t="inlineStr">
         <is>
-          <t>VICENTE DI GIORGIO</t>
+          <t>VIBES &amp; TALZ</t>
         </is>
       </c>
       <c r="V148" s="1">
-        <v>42978</v>
+        <v>43713</v>
       </c>
       <c r="W148" s="0">
         <v>0</v>
@@ -4860,15 +4860,15 @@
     </row>
     <row outlineLevel="0" r="149">
       <c r="A149" s="0">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="B149" s="0" t="inlineStr">
         <is>
-          <t>VILLAGE</t>
+          <t>VICENTE DI GIORGIO</t>
         </is>
       </c>
       <c r="V149" s="1">
-        <v>42173</v>
+        <v>42978</v>
       </c>
       <c r="W149" s="0">
         <v>0</v>
@@ -4888,15 +4888,15 @@
     </row>
     <row outlineLevel="0" r="150">
       <c r="A150" s="0">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="B150" s="0" t="inlineStr">
         <is>
-          <t>VIRA</t>
+          <t>VILLAGE</t>
         </is>
       </c>
       <c r="V150" s="1">
-        <v>42859</v>
+        <v>42173</v>
       </c>
       <c r="W150" s="0">
         <v>0</v>
@@ -4916,15 +4916,15 @@
     </row>
     <row outlineLevel="0" r="151">
       <c r="A151" s="0">
-        <v>130</v>
+        <v>64</v>
       </c>
       <c r="B151" s="0" t="inlineStr">
         <is>
-          <t>VIRA CENÁRIOS</t>
+          <t>VIRA</t>
         </is>
       </c>
       <c r="V151" s="1">
-        <v>43902</v>
+        <v>42859</v>
       </c>
       <c r="W151" s="0">
         <v>0</v>
@@ -4944,15 +4944,15 @@
     </row>
     <row outlineLevel="0" r="152">
       <c r="A152" s="0">
-        <v>154</v>
+        <v>130</v>
       </c>
       <c r="B152" s="0" t="inlineStr">
         <is>
-          <t>VIVO</t>
+          <t>VIRA CENÁRIOS</t>
         </is>
       </c>
       <c r="V152" s="1">
-        <v>44446</v>
+        <v>43902</v>
       </c>
       <c r="W152" s="0">
         <v>0</v>
@@ -4972,15 +4972,15 @@
     </row>
     <row outlineLevel="0" r="153">
       <c r="A153" s="0">
-        <v>41</v>
+        <v>154</v>
       </c>
       <c r="B153" s="0" t="inlineStr">
         <is>
-          <t>VM-OFFICE</t>
+          <t>VIVO</t>
         </is>
       </c>
       <c r="V153" s="1">
-        <v>42485</v>
+        <v>44446</v>
       </c>
       <c r="W153" s="0">
         <v>0</v>
@@ -5000,15 +5000,15 @@
     </row>
     <row outlineLevel="0" r="154">
       <c r="A154" s="0">
-        <v>94</v>
+        <v>41</v>
       </c>
       <c r="B154" s="0" t="inlineStr">
         <is>
-          <t>VODKA VOA</t>
+          <t>VM-OFFICE</t>
         </is>
       </c>
       <c r="V154" s="1">
-        <v>43507</v>
+        <v>42485</v>
       </c>
       <c r="W154" s="0">
         <v>0</v>
@@ -5028,15 +5028,15 @@
     </row>
     <row outlineLevel="0" r="155">
       <c r="A155" s="0">
-        <v>163</v>
+        <v>94</v>
       </c>
       <c r="B155" s="0" t="inlineStr">
         <is>
-          <t>VOE IDEIAS</t>
+          <t>VODKA VOA</t>
         </is>
       </c>
       <c r="V155" s="1">
-        <v>44508</v>
+        <v>43507</v>
       </c>
       <c r="W155" s="0">
         <v>0</v>
@@ -5056,15 +5056,15 @@
     </row>
     <row outlineLevel="0" r="156">
       <c r="A156" s="0">
-        <v>42</v>
+        <v>163</v>
       </c>
       <c r="B156" s="0" t="inlineStr">
         <is>
-          <t>VOID</t>
+          <t>VOE IDEIAS</t>
         </is>
       </c>
       <c r="V156" s="1">
-        <v>42501</v>
+        <v>44508</v>
       </c>
       <c r="W156" s="0">
         <v>0</v>
@@ -5084,15 +5084,15 @@
     </row>
     <row outlineLevel="0" r="157">
       <c r="A157" s="0">
-        <v>81</v>
+        <v>42</v>
       </c>
       <c r="B157" s="0" t="inlineStr">
         <is>
-          <t>WGC</t>
+          <t>VOID</t>
         </is>
       </c>
       <c r="V157" s="1">
-        <v>43060</v>
+        <v>42501</v>
       </c>
       <c r="W157" s="0">
         <v>0</v>
@@ -5112,15 +5112,15 @@
     </row>
     <row outlineLevel="0" r="158">
       <c r="A158" s="0">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="B158" s="0" t="inlineStr">
         <is>
-          <t>X3M - JUNIOR</t>
+          <t>WGC</t>
         </is>
       </c>
       <c r="V158" s="1">
-        <v>43706</v>
+        <v>43060</v>
       </c>
       <c r="W158" s="0">
         <v>0</v>
@@ -5140,29 +5140,57 @@
     </row>
     <row outlineLevel="0" r="159">
       <c r="A159" s="0">
+        <v>110</v>
+      </c>
+      <c r="B159" s="0" t="inlineStr">
+        <is>
+          <t>X3M - JUNIOR</t>
+        </is>
+      </c>
+      <c r="V159" s="1">
+        <v>43706</v>
+      </c>
+      <c r="W159" s="0">
+        <v>0</v>
+      </c>
+      <c r="X159" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y159" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA159" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB159" s="0" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="160">
+      <c r="A160" s="0">
         <v>30</v>
       </c>
-      <c r="B159" s="0" t="inlineStr">
+      <c r="B160" s="0" t="inlineStr">
         <is>
           <t>ZEH PRETIM</t>
         </is>
       </c>
-      <c r="V159" s="1">
+      <c r="V160" s="1">
         <v>42391</v>
       </c>
-      <c r="W159" s="0">
-        <v>0</v>
-      </c>
-      <c r="X159" s="0">
-        <v>0</v>
-      </c>
-      <c r="Y159" s="0">
-        <v>0</v>
-      </c>
-      <c r="AA159" s="0">
-        <v>0</v>
-      </c>
-      <c r="AB159" s="0" t="b">
+      <c r="W160" s="0">
+        <v>0</v>
+      </c>
+      <c r="X160" s="0">
+        <v>0</v>
+      </c>
+      <c r="Y160" s="0">
+        <v>0</v>
+      </c>
+      <c r="AA160" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB160" s="0" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>